<commit_message>
Updated code generator scripts supporting separated input/output port groups of cNPNZ16b_t data structure
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71059612-9AD1-4E2B-8CD8-C4C8F88E4E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F655B29-8231-4EE3-8394-B4F21147FB9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10500" tabRatio="654" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="507">
   <si>
     <t>line0</t>
   </si>
@@ -675,9 +675,6 @@
     <t>%IDENT%// Filter coefficients and input/output histories</t>
   </si>
   <si>
-    <t>%IDENT%// Feedback conditioning</t>
-  </si>
-  <si>
     <t>%IDENT%// Voltage/Average Current Mode Control Trigger handling</t>
   </si>
   <si>
@@ -1239,21 +1236,6 @@
     <t>volatile uint16_t %FILENAME_PATTERN%_Initialize(volatile %STRUCTURE_LABEL%* controller)</t>
   </si>
   <si>
-    <t>%IDENT%%IDENT%volatile unsigned agm_enable: 1; // Bit 11: when set, Adaptive Gain Modulation is enabled</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t* ptrSource; // Pointer to source register or variable where the input value is read from (e.g. ADCBUFx)</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t* ptrAltSource; // Pointer to alternate source register or variable where the alternate input value is read from (e.g. ADCBUFy)</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t* ptrTarget; // Pointer to target register or variable where the control output is written to (e.g. PCDx)</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t* ptrAltTarget; // Pointer to alternate target register or variable where the alternate control output is written to (e.g. PCDy)</t>
-  </si>
-  <si>
     <t>%IDENT%%IDENT%volatile uint16_t* ptrControlReference; // Pointer to global variable of input register holding the controller reference value (e.g. uint16_t my_ref)</t>
   </si>
   <si>
@@ -1293,9 +1275,6 @@
     <t>%IDENT%%IDENT%volatile int16_t normPostScaler; // Control output normalization factor (Q15) (R/W)</t>
   </si>
   <si>
-    <t>%IDENT%%IDENT%volatile int16_t InputOffset; // Control input source offset value (R/W)</t>
-  </si>
-  <si>
     <t>%IDENT%%IDENT%// System clamping/Anti-windup</t>
   </si>
   <si>
@@ -1317,24 +1296,12 @@
     <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t ADCTriggerBOffset; // ADC trigger #2 offset to compensate propagation delays </t>
   </si>
   <si>
-    <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t* ptrDataProviderControlInput; // Pointer to external data buffer of most recent control input </t>
-  </si>
-  <si>
-    <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t* ptrDataProviderControlError; // Pointer to external data buffer of most recent control error </t>
-  </si>
-  <si>
-    <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t* ptrDataProviderControlOutput; // Pointer to external data buffer of most recent control output </t>
-  </si>
-  <si>
     <t>%IDENT%%IDENT%volatile uint16_t CascadedFunction; // Pointer to Function which should be called at the end of the control loop</t>
   </si>
   <si>
     <t>%IDENT%%IDENT%volatile uint16_t CascadedFunParam; // Parameter of function called (can be a pointer to a data structure)</t>
   </si>
   <si>
-    <t>%IDENT%// Adaptive Gain Modulation</t>
-  </si>
-  <si>
     <t>%IDENT%// Cascaded Function Call Parameters</t>
   </si>
   <si>
@@ -1353,27 +1320,9 @@
     <t>%IDENT%} __attribute__((packed))Filter; // Filter parameters such as pointer to history and coefficient arrays and number scaling</t>
   </si>
   <si>
-    <t>%IDENT%} __attribute__((packed))Ports; // Controller  block input and output port definitions</t>
-  </si>
-  <si>
     <t>%IDENT%volatile CONTROLLER_STATUS_t status; // Control Loop Status and Control flags</t>
   </si>
   <si>
-    <t>%IDENT%%IDENT%volatile uint16_t GainModulationFactor; // Generic 16-bit wide parameter #1 for advanced control options</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t GainModulationScaler; // Generic 16-bit wide parameter #2 for advanced control options</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t GainModulationNorm;   // Generic 16-bit wide parameter #3 for advanced control options</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t AltSourceNormShift;   // Generic 16-bit wide parameter #4 for advanced control options</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile uint16_t SourceNormShift;      // Generic 16-bit wide parameter #5 for advanced control options</t>
-  </si>
-  <si>
     <t xml:space="preserve">%IDENT%%IDENT%volatile int32_t* ptrACoefficients; // Pointer to A coefficients located in X-space </t>
   </si>
   <si>
@@ -1452,18 +1401,6 @@
     <t>#ifndef __DCLD_VERSION</t>
   </si>
   <si>
-    <t>%IDENT%CONTROLLER_STATUS_AGM_DISABLE     = 0b0000000000000000,</t>
-  </si>
-  <si>
-    <t>%IDENT%CONTROLLER_STATUS_AGM_ENABLE      = 0b0000100000000000,</t>
-  </si>
-  <si>
-    <t>#define NPNZ16_STATUS_AGM_ENABLED          1</t>
-  </si>
-  <si>
-    <t>#define NPNZ16_STATUS_AGM_DISABLED         0</t>
-  </si>
-  <si>
     <t>03/25/2020;1.1.3;Added DCLD Version Key macro to cNPNZ16b.h header file, This allows to identify the library version in user code.</t>
   </si>
   <si>
@@ -1488,13 +1425,142 @@
     <t>#endif  // end of __DCLD_VERSION</t>
   </si>
   <si>
-    <t>2.0.0</t>
-  </si>
-  <si>
     <t>03/26/2020;2.0.0;Introduction of unified, 32-bit wide coefficient number format</t>
   </si>
   <si>
     <t>This scriptprovides C-source and header files for user-tailored SMPS control loops based on DSP assembly code modules templates generated using the DCLD SDK</t>
+  </si>
+  <si>
+    <t>#define NPNZ16_STATUS_AGC_ENABLED          1</t>
+  </si>
+  <si>
+    <t>#define NPNZ16_STATUS_AGC_DISABLED         0</t>
+  </si>
+  <si>
+    <t>%IDENT%CONTROLLER_STATUS_AGC_DISABLE     = 0b0000000000000000,</t>
+  </si>
+  <si>
+    <t>} __attribute__((packed))CONTROLLER_PORT_t;</t>
+  </si>
+  <si>
+    <t>line162</t>
+  </si>
+  <si>
+    <t>line163</t>
+  </si>
+  <si>
+    <t>line164</t>
+  </si>
+  <si>
+    <t>line165</t>
+  </si>
+  <si>
+    <t>line166</t>
+  </si>
+  <si>
+    <t>line167</t>
+  </si>
+  <si>
+    <t>line168</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile CONTROLLER_PORT_t Source; // Primary data input port declaration</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile CONTROLLER_PORT_t AltSource; // Secondary data input port declaration</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile CONTROLLER_PORT_t Target; // Primary data output port declaration</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile CONTROLLER_PORT_t AltTarget; // Secondary data output port declaration</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t agcScaler; // Bit-shift scaler of Adaptive Gain Modulation factor</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile fractional agcFactor; // Q15 value of Adaptive Gain Modulation factor</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile fractional agcMedian; // Q15 value of Adaptive Gain Modulation nominal operating point</t>
+  </si>
+  <si>
+    <t>%IDENT%} __attribute__((packed))GainControl; // Parameter section for advanced control options</t>
+  </si>
+  <si>
+    <t>%IDENT%// User Data Space for Advanced Control Functions</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t advParam1; // generic 16-bit wide, user-defined parameter #1 for advanced control options</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t advParam2; // generic 16-bit wide, user-defined parameter #2 for advanced control options</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t advParam3; // generic 16-bit wide, user-defined parameter #3 for advanced control options</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t advParam4; // generic 16-bit wide, user-defined parameter #4 for advanced control options</t>
+  </si>
+  <si>
+    <t>line169</t>
+  </si>
+  <si>
+    <t>line170</t>
+  </si>
+  <si>
+    <t>line171</t>
+  </si>
+  <si>
+    <t>line172</t>
+  </si>
+  <si>
+    <t>line173</t>
+  </si>
+  <si>
+    <t>%IDENT%// Adaptive Gain Control Modulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t* ptrDProvControlInput; // Pointer to external data buffer of most recent control input </t>
+  </si>
+  <si>
+    <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t* ptrDProvControlError; // Pointer to external data buffer of most recent control error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t* ptrDProvControlOutput; // Pointer to external data buffer of most recent control output </t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile int16_t AltMinOutput; // Alternate minimum output value used for clamping (R/W)</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile int16_t AltMaxOutput; // Alternate maximum output value used for clamping (R/W)</t>
+  </si>
+  <si>
+    <t>2.0.1</t>
+  </si>
+  <si>
+    <t>03/27/2020;2.0.1;Separated input and output ports and added individual normalization scaling parameters</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile unsigned agc_enabled: 1; // Bit 11: when set, Adaptive Gain Control Modulation is enabled</t>
+  </si>
+  <si>
+    <t>%IDENT%volatile uint16_t* ptrAddress; // Pointer to register or variable where the value is read from (e.g. ADCBUFx) or written to (e.g. PGxDC)</t>
+  </si>
+  <si>
+    <t>%IDENT%volatile uint16_t  NormScaler; // Bit-shift scaler of the Q15 normalization factor</t>
+  </si>
+  <si>
+    <t>%IDENT%volatile fractional NormFactor; // Q15 normalization factor</t>
+  </si>
+  <si>
+    <t>%IDENT%volatile uint16_t  Offset; // Value/signal offset of this port</t>
+  </si>
+  <si>
+    <t>%IDENT%CONTROLLER_STATUS_AGC_ENABLED     = 0b0000100000000000,</t>
+  </si>
+  <si>
+    <t>%IDENT%} __attribute__((packed))Ports; // Controller block input and output port definitions</t>
   </si>
 </sst>
 </file>
@@ -1929,10 +1995,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EEA387-D56E-491B-9839-D10FC585EB9A}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,69 +2010,69 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>484</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>482</v>
+        <v>498</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C6" s="7">
-        <v>43916</v>
+        <v>43917</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2019,8 +2085,8 @@
         <v>162</v>
       </c>
       <c r="C9" s="3">
-        <f>COUNTA(A10:A18)</f>
-        <v>8</v>
+        <f>COUNTA(A10:A19)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2031,7 +2097,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2042,7 +2108,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2053,7 +2119,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2064,7 +2130,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2075,7 +2141,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2086,7 +2152,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2097,7 +2163,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2108,7 +2174,18 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>483</v>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -2121,9 +2198,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2134,7 +2209,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2170,7 +2245,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2181,7 +2256,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2192,7 +2267,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2203,7 +2278,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2214,7 +2289,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2225,7 +2300,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2236,7 +2311,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2247,7 +2322,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2258,7 +2333,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2269,7 +2344,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2280,7 +2355,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2291,7 +2366,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2302,7 +2377,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2313,7 +2388,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2324,7 +2399,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2335,7 +2410,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2359,42 +2434,42 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -2405,11 +2480,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798E1EF1-7DA6-47D5-9A26-6753C89CA0C2}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:B164"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2434,7 +2507,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,7 +2573,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2610,7 +2683,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2621,7 +2694,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2632,7 +2705,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2643,7 +2716,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2654,7 +2727,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2665,7 +2738,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2742,7 +2815,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2753,7 +2826,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2764,7 +2837,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2775,7 +2848,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2786,7 +2859,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2797,7 +2870,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2885,7 +2958,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2896,7 +2969,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2907,7 +2980,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2918,7 +2991,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2929,7 +3002,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2940,7 +3013,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2951,7 +3024,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2962,7 +3035,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>471</v>
+        <v>505</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2973,7 +3046,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2984,7 +3057,7 @@
         <v>162</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2995,7 +3068,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3006,7 +3079,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3017,7 +3090,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3028,7 +3101,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3039,7 +3112,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3050,7 +3123,7 @@
         <v>162</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3226,7 +3299,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>399</v>
+        <v>500</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3237,7 +3310,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3248,7 +3321,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3270,7 +3343,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3336,7 +3409,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>208</v>
+        <v>501</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3347,7 +3420,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>438</v>
+        <v>502</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3358,7 +3431,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>173</v>
+        <v>503</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3369,7 +3442,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>209</v>
+        <v>504</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3380,7 +3453,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>191</v>
+        <v>466</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3391,7 +3464,7 @@
         <v>162</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>400</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3402,7 +3475,7 @@
         <v>162</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>401</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3413,7 +3486,7 @@
         <v>162</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>402</v>
+        <v>208</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3424,7 +3497,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3435,7 +3508,7 @@
         <v>162</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>404</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3446,7 +3519,7 @@
         <v>162</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>437</v>
+        <v>209</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3457,7 +3530,7 @@
         <v>162</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3468,7 +3541,7 @@
         <v>162</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>210</v>
+        <v>474</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3479,7 +3552,7 @@
         <v>162</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>191</v>
+        <v>475</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3490,7 +3563,7 @@
         <v>162</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>444</v>
+        <v>476</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3501,7 +3574,7 @@
         <v>162</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>445</v>
+        <v>477</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3512,7 +3585,7 @@
         <v>162</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -3523,7 +3596,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>406</v>
+        <v>506</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3545,7 +3618,7 @@
         <v>162</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>407</v>
+        <v>210</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3556,7 +3629,7 @@
         <v>162</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>408</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3567,7 +3640,7 @@
         <v>162</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>409</v>
+        <v>427</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3578,7 +3651,7 @@
         <v>162</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3589,7 +3662,7 @@
         <v>162</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3600,7 +3673,7 @@
         <v>162</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>173</v>
+        <v>400</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3611,7 +3684,7 @@
         <v>162</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>412</v>
+        <v>173</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3622,7 +3695,7 @@
         <v>162</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3633,7 +3706,7 @@
         <v>162</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3644,7 +3717,7 @@
         <v>162</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3655,7 +3728,7 @@
         <v>162</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3666,7 +3739,7 @@
         <v>162</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>436</v>
+        <v>405</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3688,7 +3761,7 @@
         <v>162</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>211</v>
+        <v>406</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3699,7 +3772,7 @@
         <v>162</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>191</v>
+        <v>407</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3710,7 +3783,7 @@
         <v>162</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3721,7 +3794,7 @@
         <v>162</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>173</v>
+        <v>409</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3732,7 +3805,7 @@
         <v>162</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3743,7 +3816,7 @@
         <v>162</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3754,7 +3827,7 @@
         <v>162</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>420</v>
+        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3765,7 +3838,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3776,7 +3849,7 @@
         <v>162</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3787,7 +3860,7 @@
         <v>162</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>212</v>
+        <v>412</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3798,7 +3871,7 @@
         <v>162</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>191</v>
+        <v>413</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3809,7 +3882,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>421</v>
+        <v>496</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3820,7 +3893,7 @@
         <v>162</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>422</v>
+        <v>497</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3831,7 +3904,7 @@
         <v>162</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3842,7 +3915,7 @@
         <v>162</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>424</v>
+        <v>173</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -3853,7 +3926,7 @@
         <v>162</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>434</v>
+        <v>211</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -3864,7 +3937,7 @@
         <v>162</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -3875,7 +3948,7 @@
         <v>162</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>213</v>
+        <v>414</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3886,7 +3959,7 @@
         <v>162</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>191</v>
+        <v>415</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3897,7 +3970,7 @@
         <v>162</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -3908,7 +3981,7 @@
         <v>162</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3919,7 +3992,7 @@
         <v>162</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -3930,7 +4003,7 @@
         <v>162</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>433</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -3941,7 +4014,7 @@
         <v>162</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -3952,7 +4025,7 @@
         <v>162</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>431</v>
+        <v>191</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -3963,7 +4036,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>191</v>
+        <v>493</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -3974,7 +4047,7 @@
         <v>162</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>428</v>
+        <v>494</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -3985,7 +4058,7 @@
         <v>162</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>429</v>
+        <v>495</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -3996,7 +4069,7 @@
         <v>162</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4018,7 +4091,7 @@
         <v>162</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -4040,7 +4113,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4051,7 +4124,7 @@
         <v>162</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -4062,7 +4135,7 @@
         <v>162</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -4073,7 +4146,7 @@
         <v>162</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>442</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -4084,7 +4157,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>443</v>
+        <v>492</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -4095,7 +4168,7 @@
         <v>162</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>462</v>
+        <v>191</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -4106,7 +4179,7 @@
         <v>162</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>173</v>
+        <v>478</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -4117,7 +4190,7 @@
         <v>162</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>214</v>
+        <v>479</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -4128,7 +4201,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>173</v>
+        <v>480</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4139,7 +4212,7 @@
         <v>162</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>460</v>
+        <v>481</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4150,7 +4223,7 @@
         <v>162</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>461</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -4161,7 +4234,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>173</v>
+        <v>482</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -4172,7 +4245,7 @@
         <v>162</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -4183,7 +4256,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>215</v>
+        <v>483</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4194,7 +4267,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>216</v>
+        <v>484</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -4205,7 +4278,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>215</v>
+        <v>485</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4216,6 +4289,138 @@
         <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C176" s="2" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4231,9 +4436,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4244,7 +4447,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4280,7 +4483,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4291,7 +4494,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4302,7 +4505,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4313,7 +4516,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4324,7 +4527,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4335,7 +4538,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4346,7 +4549,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4357,7 +4560,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4368,7 +4571,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4379,7 +4582,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4390,7 +4593,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4401,7 +4604,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4412,7 +4615,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4423,7 +4626,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4434,7 +4637,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4445,7 +4648,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4456,7 +4659,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4467,7 +4670,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4478,7 +4681,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4500,7 +4703,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4511,7 +4714,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4588,7 +4791,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -4610,7 +4813,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4621,7 +4824,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4632,7 +4835,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4643,7 +4846,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4654,7 +4857,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4665,7 +4868,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4676,7 +4879,7 @@
         <v>162</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4687,7 +4890,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4698,7 +4901,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4709,7 +4912,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4720,7 +4923,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4731,7 +4934,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4742,7 +4945,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4753,7 +4956,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4764,7 +4967,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4775,7 +4978,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -4786,7 +4989,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4797,7 +5000,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4819,7 +5022,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4830,7 +5033,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -4841,7 +5044,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -4852,7 +5055,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4863,7 +5066,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -4896,7 +5099,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -4918,7 +5121,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -4929,7 +5132,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4940,7 +5143,7 @@
         <v>162</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4962,7 +5165,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -4973,7 +5176,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4984,7 +5187,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4995,7 +5198,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -5017,7 +5220,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -5028,7 +5231,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -5039,7 +5242,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -5050,7 +5253,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -5072,7 +5275,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -5083,7 +5286,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -5094,7 +5297,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -5105,7 +5308,7 @@
         <v>162</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -5116,7 +5319,7 @@
         <v>162</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -5127,7 +5330,7 @@
         <v>162</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -5149,7 +5352,7 @@
         <v>162</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -5160,7 +5363,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -5171,7 +5374,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -5182,7 +5385,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -5215,7 +5418,7 @@
         <v>162</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -5248,7 +5451,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -5259,7 +5462,7 @@
         <v>162</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -5270,7 +5473,7 @@
         <v>162</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -5296,9 +5499,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5309,7 +5510,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5334,7 +5535,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5345,7 +5546,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5356,7 +5557,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5367,7 +5568,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5378,7 +5579,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5389,7 +5590,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5400,7 +5601,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5411,7 +5612,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5422,7 +5623,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5433,7 +5634,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5444,7 +5645,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5455,7 +5656,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5466,7 +5667,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5477,7 +5678,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5488,7 +5689,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5499,7 +5700,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5510,7 +5711,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5521,7 +5722,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5532,7 +5733,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5543,7 +5744,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5565,7 +5766,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5587,7 +5788,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5598,7 +5799,7 @@
         <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5609,7 +5810,7 @@
         <v>162</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5620,7 +5821,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5631,7 +5832,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5642,7 +5843,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5653,7 +5854,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5664,7 +5865,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5675,7 +5876,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5686,7 +5887,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5697,7 +5898,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5708,7 +5909,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5719,7 +5920,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5730,7 +5931,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5752,7 +5953,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5763,7 +5964,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5774,7 +5975,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5796,7 +5997,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5807,7 +6008,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5818,7 +6019,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5840,7 +6041,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -5851,7 +6052,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -5862,7 +6063,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -5873,7 +6074,7 @@
         <v>162</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -5884,7 +6085,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -5895,7 +6096,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -5906,7 +6107,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5917,7 +6118,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -5928,7 +6129,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5939,7 +6140,7 @@
         <v>162</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -5950,10 +6151,10 @@
         <v>162</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D59" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -5964,7 +6165,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -5975,7 +6176,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -5986,7 +6187,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6008,10 +6209,10 @@
         <v>162</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D64" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6022,7 +6223,7 @@
         <v>162</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6033,7 +6234,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6044,7 +6245,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6066,7 +6267,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6077,7 +6278,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6088,7 +6289,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6099,7 +6300,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6110,7 +6311,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6132,7 +6333,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6154,7 +6355,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6190,7 +6391,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6209,13 +6410,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -6228,8 +6429,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:B69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6241,7 +6442,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6266,7 +6467,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6277,7 +6478,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6288,7 +6489,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6299,7 +6500,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6310,7 +6511,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6321,7 +6522,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6332,7 +6533,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6343,7 +6544,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6354,7 +6555,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6365,7 +6566,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6387,7 +6588,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6398,7 +6599,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6409,7 +6610,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6420,7 +6621,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6431,7 +6632,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6442,7 +6643,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6453,7 +6654,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6464,7 +6665,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6475,7 +6676,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6486,7 +6687,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6497,7 +6698,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6508,7 +6709,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6519,7 +6720,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6530,7 +6731,7 @@
         <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6552,7 +6753,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6563,7 +6764,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6574,7 +6775,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6585,7 +6786,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6596,7 +6797,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6607,7 +6808,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6618,7 +6819,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6629,7 +6830,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6640,7 +6841,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6651,7 +6852,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6662,7 +6863,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6673,7 +6874,7 @@
         <v>162</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6684,7 +6885,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6695,7 +6896,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6706,7 +6907,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6717,7 +6918,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6728,7 +6929,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -6739,7 +6940,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6750,7 +6951,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6761,7 +6962,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>458</v>
+        <v>441</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6772,7 +6973,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6783,7 +6984,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6794,7 +6995,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6816,7 +7017,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6827,7 +7028,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6838,7 +7039,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6849,7 +7050,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6860,7 +7061,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6882,7 +7083,7 @@
         <v>162</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6893,7 +7094,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6904,7 +7105,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6915,7 +7116,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6926,7 +7127,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -6959,7 +7160,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6970,7 +7171,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6981,7 +7182,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed formating and comments in code generator script files
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F655B29-8231-4EE3-8394-B4F21147FB9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73D94F1-D45E-49DC-9300-617D12DB5411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="3" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -1275,9 +1275,6 @@
     <t>%IDENT%%IDENT%volatile int16_t normPostScaler; // Control output normalization factor (Q15) (R/W)</t>
   </si>
   <si>
-    <t>%IDENT%%IDENT%// System clamping/Anti-windup</t>
-  </si>
-  <si>
     <t>%IDENT%%IDENT%volatile int16_t MinOutput; // Minimum output value used for clamping (R/W)</t>
   </si>
   <si>
@@ -1561,6 +1558,9 @@
   </si>
   <si>
     <t>%IDENT%} __attribute__((packed))Ports; // Controller block input and output port definitions</t>
+  </si>
+  <si>
+    <t>%IDENT%// System clamping/Anti-windup</t>
   </si>
 </sst>
 </file>
@@ -1997,9 +1997,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2034,7 +2032,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2056,7 +2054,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2119,7 +2117,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2130,7 +2128,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2141,7 +2139,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2152,7 +2150,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2163,7 +2161,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2174,7 +2172,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2185,7 +2183,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -2355,7 +2353,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2482,7 +2480,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2573,7 +2573,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2683,7 +2683,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2716,7 +2716,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3035,7 +3035,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3420,7 +3420,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3431,7 +3431,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3442,7 +3442,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3453,7 +3453,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3497,7 +3497,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3541,7 +3541,7 @@
         <v>162</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3552,7 +3552,7 @@
         <v>162</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3563,7 +3563,7 @@
         <v>162</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3574,7 +3574,7 @@
         <v>162</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3640,7 +3640,7 @@
         <v>162</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3651,7 +3651,7 @@
         <v>162</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3816,7 +3816,7 @@
         <v>162</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3838,7 +3838,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>411</v>
+        <v>506</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3860,7 +3860,7 @@
         <v>162</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3871,7 +3871,7 @@
         <v>162</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3882,7 +3882,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3893,7 +3893,7 @@
         <v>162</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3904,7 +3904,7 @@
         <v>162</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3948,7 +3948,7 @@
         <v>162</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3959,7 +3959,7 @@
         <v>162</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3970,7 +3970,7 @@
         <v>162</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -3981,7 +3981,7 @@
         <v>162</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3992,7 +3992,7 @@
         <v>162</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
         <v>162</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -4058,7 +4058,7 @@
         <v>162</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>162</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4091,7 +4091,7 @@
         <v>162</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -4113,7 +4113,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4124,7 +4124,7 @@
         <v>162</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -4135,7 +4135,7 @@
         <v>162</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -4157,7 +4157,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -4179,7 +4179,7 @@
         <v>162</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -4190,7 +4190,7 @@
         <v>162</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -4201,7 +4201,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4212,7 +4212,7 @@
         <v>162</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4234,7 +4234,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -4256,7 +4256,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4267,7 +4267,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -4278,7 +4278,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4289,23 +4289,23 @@
         <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>162</v>
@@ -4316,7 +4316,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>162</v>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>162</v>
@@ -4338,29 +4338,29 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>162</v>
@@ -4371,7 +4371,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>162</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>162</v>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>162</v>
@@ -4404,7 +4404,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>162</v>
@@ -4415,7 +4415,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>162</v>
@@ -4637,7 +4637,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5700,7 +5700,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6786,7 +6786,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6797,7 +6797,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6808,7 +6808,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6819,7 +6819,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6830,7 +6830,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6841,7 +6841,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6852,7 +6852,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6863,7 +6863,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6885,7 +6885,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6896,7 +6896,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6907,7 +6907,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6918,7 +6918,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -7028,7 +7028,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Renamed cNPNZ16b_t data structure group 'TriggerControl' to 'ADCTriggerControl'
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73D94F1-D45E-49DC-9300-617D12DB5411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C008B505-461F-45AE-9D82-B24176036AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="3" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="7" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="508">
   <si>
     <t>line0</t>
   </si>
@@ -1308,9 +1308,6 @@
     <t>%IDENT%} __attribute__((packed))DataProviders; // Automated data sources pushing data points to user-defined variables</t>
   </si>
   <si>
-    <t>%IDENT%} __attribute__((packed))TriggerControl; // Automatic ADC trigger placement options for ADC Trigger A and B</t>
-  </si>
-  <si>
     <t>%IDENT%} __attribute__((packed))Limits; // Input and output clamping values</t>
   </si>
   <si>
@@ -1533,9 +1530,6 @@
     <t>%IDENT%%IDENT%volatile int16_t AltMaxOutput; // Alternate maximum output value used for clamping (R/W)</t>
   </si>
   <si>
-    <t>2.0.1</t>
-  </si>
-  <si>
     <t>03/27/2020;2.0.1;Separated input and output ports and added individual normalization scaling parameters</t>
   </si>
   <si>
@@ -1561,6 +1555,15 @@
   </si>
   <si>
     <t>%IDENT%// System clamping/Anti-windup</t>
+  </si>
+  <si>
+    <t>%IDENT%} __attribute__((packed))ADCTriggerControl; // Automatic ADC trigger placement options for ADC Trigger A and B</t>
+  </si>
+  <si>
+    <t>2.0.2</t>
+  </si>
+  <si>
+    <t>03/30/2020;2.0.2;Renamed data structure group 'TriggerControl' to 'ADC TriggerControl'</t>
   </si>
 </sst>
 </file>
@@ -1995,7 +1998,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EEA387-D56E-491B-9839-D10FC585EB9A}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2032,7 +2035,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,7 +2057,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>497</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2065,7 +2068,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="7">
-        <v>43917</v>
+        <v>43920</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -2083,8 +2086,8 @@
         <v>162</v>
       </c>
       <c r="C9" s="3">
-        <f>COUNTA(A10:A19)</f>
-        <v>9</v>
+        <f>COUNTA(A10:A20)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2117,7 +2120,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2128,7 +2131,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2139,7 +2142,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2150,7 +2153,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2161,7 +2164,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2172,7 +2175,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2183,7 +2186,18 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -2353,7 +2367,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2480,8 +2494,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2587,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2683,7 +2697,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2694,7 +2708,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2705,7 +2719,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2716,7 +2730,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2727,7 +2741,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2738,7 +2752,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2815,7 +2829,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2826,7 +2840,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3024,7 +3038,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3035,7 +3049,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3299,7 +3313,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3343,7 +3357,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3409,7 +3423,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3420,7 +3434,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3431,7 +3445,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3442,7 +3456,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3453,7 +3467,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3497,7 +3511,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3541,7 +3555,7 @@
         <v>162</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3552,7 +3566,7 @@
         <v>162</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3563,7 +3577,7 @@
         <v>162</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3574,7 +3588,7 @@
         <v>162</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3596,7 +3610,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3640,7 +3654,7 @@
         <v>162</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3651,7 +3665,7 @@
         <v>162</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3816,7 +3830,7 @@
         <v>162</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3838,7 +3852,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3882,7 +3896,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3893,7 +3907,7 @@
         <v>162</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3904,7 +3918,7 @@
         <v>162</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3992,7 +4006,7 @@
         <v>162</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>422</v>
+        <v>505</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -4036,7 +4050,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,7 +4061,7 @@
         <v>162</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -4058,7 +4072,7 @@
         <v>162</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -4157,7 +4171,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -4179,7 +4193,7 @@
         <v>162</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -4190,7 +4204,7 @@
         <v>162</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -4201,7 +4215,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4212,7 +4226,7 @@
         <v>162</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4234,7 +4248,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -4256,7 +4270,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4267,7 +4281,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -4278,7 +4292,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4289,23 +4303,23 @@
         <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>162</v>
@@ -4316,7 +4330,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>162</v>
@@ -4327,7 +4341,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>162</v>
@@ -4338,29 +4352,29 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>162</v>
@@ -4371,7 +4385,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>162</v>
@@ -4382,7 +4396,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>162</v>
@@ -4393,7 +4407,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>162</v>
@@ -4404,7 +4418,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>162</v>
@@ -4415,7 +4429,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>162</v>
@@ -4637,7 +4651,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5700,7 +5714,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6429,7 +6443,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6786,7 +6800,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6797,7 +6811,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6808,7 +6822,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6819,7 +6833,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6830,7 +6844,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6841,7 +6855,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6852,7 +6866,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6863,7 +6877,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6885,7 +6899,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6896,7 +6910,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6907,7 +6921,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6918,7 +6932,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6962,7 +6976,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -7028,7 +7042,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code generator scripts containing P-Term controller code templates
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C008B505-461F-45AE-9D82-B24176036AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B9A289-3AA6-47FF-8A10-D4B00C0471C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="7" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="3" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="514">
   <si>
     <t>line0</t>
   </si>
@@ -849,9 +849,6 @@
     <t>%IDENT%%IDENT%volatile %HISTORY_DATA_TYPE% ctrl_output // user-defined, constant control output history value</t>
   </si>
   <si>
-    <t>// Calls the %FILENAME_PATTERN% controller object</t>
-  </si>
-  <si>
     <t>extern void %FILENAME_PATTERN%_Update( // Calls the %FILTER_ORDER%P%FILTER_ORDER%Z controller (Assembly)</t>
   </si>
   <si>
@@ -1293,9 +1290,6 @@
     <t xml:space="preserve">%IDENT%%IDENT%volatile uint16_t ADCTriggerBOffset; // ADC trigger #2 offset to compensate propagation delays </t>
   </si>
   <si>
-    <t>%IDENT%%IDENT%volatile uint16_t CascadedFunction; // Pointer to Function which should be called at the end of the control loop</t>
-  </si>
-  <si>
     <t>%IDENT%%IDENT%volatile uint16_t CascadedFunParam; // Parameter of function called (can be a pointer to a data structure)</t>
   </si>
   <si>
@@ -1560,10 +1554,34 @@
     <t>%IDENT%} __attribute__((packed))ADCTriggerControl; // Automatic ADC trigger placement options for ADC Trigger A and B</t>
   </si>
   <si>
-    <t>2.0.2</t>
-  </si>
-  <si>
     <t>03/30/2020;2.0.2;Renamed data structure group 'TriggerControl' to 'ADC TriggerControl'</t>
+  </si>
+  <si>
+    <t>// Calls the %FILENAME_PATTERN% control loop</t>
+  </si>
+  <si>
+    <t>extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)</t>
+  </si>
+  <si>
+    <t>// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions</t>
+  </si>
+  <si>
+    <t>// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY.</t>
+  </si>
+  <si>
+    <t>// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION</t>
+  </si>
+  <si>
+    <t>// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS</t>
+  </si>
+  <si>
+    <t>2.0.3</t>
+  </si>
+  <si>
+    <t>03/31/2020;2.0.3;Added P-Term controller for plant transfer function measurement support</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t ptrCascadedFunction; // Pointer to Function which should be called at the end of the control loop</t>
   </si>
 </sst>
 </file>
@@ -1998,7 +2016,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EEA387-D56E-491B-9839-D10FC585EB9A}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2011,69 +2029,69 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C6" s="7">
-        <v>43920</v>
+        <v>43921</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2086,8 +2104,8 @@
         <v>162</v>
       </c>
       <c r="C9" s="3">
-        <f>COUNTA(A10:A20)</f>
-        <v>10</v>
+        <f>COUNTA(A10:A21)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2098,7 +2116,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2109,7 +2127,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2120,7 +2138,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,7 +2149,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2160,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,7 +2171,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,7 +2182,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2193,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,7 +2204,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2197,7 +2215,18 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -2221,7 +2250,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2257,7 +2286,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2297,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2308,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2319,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2330,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2341,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2352,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2363,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2374,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,7 +2385,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2396,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2378,7 +2407,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2389,7 +2418,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,7 +2429,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,7 +2440,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,7 +2451,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2446,42 +2475,42 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2494,9 +2523,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2587,7 +2614,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2697,7 +2724,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2708,7 +2735,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2719,7 +2746,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2730,7 +2757,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2741,7 +2768,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2752,7 +2779,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,7 +2856,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2840,7 +2867,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2851,7 +2878,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2862,7 +2889,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2972,7 +2999,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2983,7 +3010,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2994,7 +3021,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3005,7 +3032,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3016,7 +3043,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3027,7 +3054,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3038,7 +3065,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3049,7 +3076,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3060,7 +3087,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3071,7 +3098,7 @@
         <v>162</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3082,7 +3109,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3093,7 +3120,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3104,7 +3131,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3115,7 +3142,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3126,7 +3153,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3137,7 +3164,7 @@
         <v>162</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3313,7 +3340,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3324,7 +3351,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3335,7 +3362,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3357,7 +3384,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3423,7 +3450,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3434,7 +3461,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3445,7 +3472,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3456,7 +3483,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3467,7 +3494,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3511,7 +3538,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3555,7 +3582,7 @@
         <v>162</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3566,7 +3593,7 @@
         <v>162</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3577,7 +3604,7 @@
         <v>162</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3588,7 +3615,7 @@
         <v>162</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3599,7 +3626,7 @@
         <v>162</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -3610,7 +3637,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3654,7 +3681,7 @@
         <v>162</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3665,7 +3692,7 @@
         <v>162</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3676,7 +3703,7 @@
         <v>162</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3687,7 +3714,7 @@
         <v>162</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3709,7 +3736,7 @@
         <v>162</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3720,7 +3747,7 @@
         <v>162</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3731,7 +3758,7 @@
         <v>162</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3742,7 +3769,7 @@
         <v>162</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3753,7 +3780,7 @@
         <v>162</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3775,7 +3802,7 @@
         <v>162</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3786,7 +3813,7 @@
         <v>162</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,7 +3824,7 @@
         <v>162</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3808,7 +3835,7 @@
         <v>162</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3819,7 +3846,7 @@
         <v>162</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3830,7 +3857,7 @@
         <v>162</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3852,7 +3879,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,7 +3901,7 @@
         <v>162</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,7 +3912,7 @@
         <v>162</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3896,7 +3923,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3907,7 +3934,7 @@
         <v>162</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3918,7 +3945,7 @@
         <v>162</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3962,7 +3989,7 @@
         <v>162</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3973,7 +4000,7 @@
         <v>162</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3984,7 +4011,7 @@
         <v>162</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -3995,7 +4022,7 @@
         <v>162</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -4006,7 +4033,7 @@
         <v>162</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -4050,7 +4077,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4061,7 +4088,7 @@
         <v>162</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -4072,7 +4099,7 @@
         <v>162</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -4083,7 +4110,7 @@
         <v>162</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4105,7 +4132,7 @@
         <v>162</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -4127,7 +4154,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>417</v>
+        <v>513</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4138,7 +4165,7 @@
         <v>162</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -4149,7 +4176,7 @@
         <v>162</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -4171,7 +4198,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -4193,7 +4220,7 @@
         <v>162</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -4204,7 +4231,7 @@
         <v>162</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -4215,7 +4242,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4226,7 +4253,7 @@
         <v>162</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4248,7 +4275,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -4270,7 +4297,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4281,7 +4308,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -4292,7 +4319,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4303,23 +4330,23 @@
         <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>162</v>
@@ -4330,7 +4357,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>162</v>
@@ -4341,7 +4368,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>162</v>
@@ -4352,29 +4379,29 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>162</v>
@@ -4385,7 +4412,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>162</v>
@@ -4396,7 +4423,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>162</v>
@@ -4407,7 +4434,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>162</v>
@@ -4418,7 +4445,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>162</v>
@@ -4429,7 +4456,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>162</v>
@@ -4448,9 +4475,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C06CF0-653A-4427-B7AE-138E1BDF5DAA}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4475,7 +4504,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4651,7 +4680,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5190,7 +5219,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5366,7 +5395,7 @@
         <v>162</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>269</v>
+        <v>505</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -5377,7 +5406,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -5421,7 +5450,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>173</v>
+        <v>507</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -5432,7 +5461,7 @@
         <v>162</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>271</v>
+        <v>508</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -5443,7 +5472,7 @@
         <v>162</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>173</v>
+        <v>510</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -5454,7 +5483,7 @@
         <v>162</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>173</v>
+        <v>509</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -5465,7 +5494,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>214</v>
+        <v>506</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -5476,7 +5505,7 @@
         <v>162</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -5487,7 +5516,7 @@
         <v>162</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>214</v>
+        <v>261</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -5498,6 +5527,94 @@
         <v>162</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5524,7 +5641,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5549,7 +5666,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5571,7 +5688,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5582,7 +5699,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5593,7 +5710,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5604,7 +5721,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5692,7 +5809,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5714,7 +5831,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5725,7 +5842,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5758,7 +5875,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5780,7 +5897,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5802,7 +5919,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5824,7 +5941,7 @@
         <v>162</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5835,7 +5952,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5846,7 +5963,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5868,7 +5985,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5879,7 +5996,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5890,7 +6007,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5912,7 +6029,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5923,7 +6040,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5934,7 +6051,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5945,7 +6062,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5967,7 +6084,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5978,7 +6095,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5989,7 +6106,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6011,7 +6128,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -6022,7 +6139,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6033,7 +6150,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6055,7 +6172,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6066,7 +6183,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6077,7 +6194,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6099,7 +6216,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6110,7 +6227,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6132,7 +6249,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -6143,7 +6260,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -6154,7 +6271,7 @@
         <v>162</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6165,10 +6282,10 @@
         <v>162</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D59" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6190,7 +6307,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6201,7 +6318,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6223,10 +6340,10 @@
         <v>162</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D64" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6248,7 +6365,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6259,7 +6376,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6281,7 +6398,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6292,7 +6409,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6303,7 +6420,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6314,7 +6431,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6325,7 +6442,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6347,7 +6464,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6369,7 +6486,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6405,7 +6522,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6424,13 +6541,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -6443,7 +6560,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6456,7 +6573,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6481,7 +6598,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6492,7 +6609,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6503,7 +6620,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6514,7 +6631,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6525,7 +6642,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6536,7 +6653,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6547,7 +6664,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6558,7 +6675,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6569,7 +6686,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6580,7 +6697,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6602,7 +6719,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6613,7 +6730,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6624,7 +6741,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6635,7 +6752,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6646,7 +6763,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6657,7 +6774,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6668,7 +6785,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6679,7 +6796,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6690,7 +6807,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6701,7 +6818,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6712,7 +6829,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6723,7 +6840,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6745,7 +6862,7 @@
         <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6767,7 +6884,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6778,7 +6895,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6789,7 +6906,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6800,7 +6917,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6811,7 +6928,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6822,7 +6939,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6833,7 +6950,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6844,7 +6961,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6855,7 +6972,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6866,7 +6983,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6877,7 +6994,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6888,7 +7005,7 @@
         <v>162</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6899,7 +7016,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6910,7 +7027,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6921,7 +7038,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6932,7 +7049,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6943,7 +7060,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -6954,7 +7071,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6965,7 +7082,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6976,7 +7093,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6987,7 +7104,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6998,7 +7115,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -7009,7 +7126,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -7031,7 +7148,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -7042,7 +7159,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -7053,7 +7170,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -7064,7 +7181,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -7075,7 +7192,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -7097,7 +7214,7 @@
         <v>162</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -7108,7 +7225,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -7119,7 +7236,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -7130,7 +7247,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -7141,7 +7258,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added first Conditional Token to code generator routine
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B9A289-3AA6-47FF-8A10-D4B00C0471C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC37677-DD4C-4345-9A3F-2E234C3C1840}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="3" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="1" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="519">
   <si>
     <t>line0</t>
   </si>
@@ -1560,21 +1560,6 @@
     <t>// Calls the %FILENAME_PATTERN% control loop</t>
   </si>
   <si>
-    <t>extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)</t>
-  </si>
-  <si>
-    <t>// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions</t>
-  </si>
-  <si>
-    <t>// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY.</t>
-  </si>
-  <si>
-    <t>// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION</t>
-  </si>
-  <si>
-    <t>// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS</t>
-  </si>
-  <si>
     <t>2.0.3</t>
   </si>
   <si>
@@ -1582,6 +1567,36 @@
   </si>
   <si>
     <t>%IDENT%%IDENT%volatile uint16_t ptrCascadedFunction; // Pointer to Function which should be called at the end of the control loop</t>
+  </si>
+  <si>
+    <t>[option_ids]</t>
+  </si>
+  <si>
+    <t>%{(101)}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions</t>
+  </si>
+  <si>
+    <t>%{(101)}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY.</t>
+  </si>
+  <si>
+    <t>%{(101)}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS</t>
+  </si>
+  <si>
+    <t>%{(101)}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION</t>
+  </si>
+  <si>
+    <t>%{(101)}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)</t>
+  </si>
+  <si>
+    <t>%{(101)}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object</t>
+  </si>
+  <si>
+    <t>%{(101)}%%IDENT%);</t>
+  </si>
+  <si>
+    <t>%{(101)}%%EMPTY%</t>
+  </si>
+  <si>
+    <t>%{(101)}%;pterm_enable</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2090,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2226,7 +2241,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -2237,9 +2252,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14C6232-5B4B-4D64-8489-325A578CCED2}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2263,8 +2280,8 @@
         <v>162</v>
       </c>
       <c r="C2" s="3">
-        <f>COUNTA(A:A)-2</f>
-        <v>17</v>
+        <f>COUNTA(A2:A20)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2452,6 +2469,36 @@
       </c>
       <c r="C19" s="1" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="3">
+        <f>COUNTA(A23:A30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -2523,7 +2570,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4154,7 +4201,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4478,7 +4525,7 @@
   <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5450,7 +5497,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -5461,7 +5508,7 @@
         <v>162</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -5472,7 +5519,7 @@
         <v>162</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -5483,7 +5530,7 @@
         <v>162</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -5494,7 +5541,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -5505,7 +5552,7 @@
         <v>162</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>260</v>
+        <v>515</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -5516,7 +5563,7 @@
         <v>162</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>261</v>
+        <v>516</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -5527,7 +5574,7 @@
         <v>162</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>173</v>
+        <v>517</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -5630,7 +5677,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Synched tokens of C-code and assembly generator scripts.
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC37677-DD4C-4345-9A3F-2E234C3C1840}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F72C68-6AD5-435D-8B85-3EF918AE5AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="1" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="7" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="550">
   <si>
     <t>line0</t>
   </si>
@@ -1560,9 +1560,6 @@
     <t>// Calls the %FILENAME_PATTERN% control loop</t>
   </si>
   <si>
-    <t>2.0.3</t>
-  </si>
-  <si>
     <t>03/31/2020;2.0.3;Added P-Term controller for plant transfer function measurement support</t>
   </si>
   <si>
@@ -1572,31 +1569,127 @@
     <t>[option_ids]</t>
   </si>
   <si>
-    <t>%{(101)}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions</t>
-  </si>
-  <si>
-    <t>%{(101)}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY.</t>
-  </si>
-  <si>
-    <t>%{(101)}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS</t>
-  </si>
-  <si>
-    <t>%{(101)}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION</t>
-  </si>
-  <si>
-    <t>%{(101)}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)</t>
-  </si>
-  <si>
-    <t>%{(101)}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object</t>
-  </si>
-  <si>
-    <t>%{(101)}%%IDENT%);</t>
-  </si>
-  <si>
-    <t>%{(101)}%%EMPTY%</t>
-  </si>
-  <si>
-    <t>%{(101)}%;pterm_enable</t>
+    <t>token_id</t>
+  </si>
+  <si>
+    <t>token_key</t>
+  </si>
+  <si>
+    <t>context_management</t>
+  </si>
+  <si>
+    <t>option_add_p-term</t>
+  </si>
+  <si>
+    <t>context_shadow</t>
+  </si>
+  <si>
+    <t>context_mac_wreg</t>
+  </si>
+  <si>
+    <t>context_acc</t>
+  </si>
+  <si>
+    <t>context_acc_a</t>
+  </si>
+  <si>
+    <t>context_acc_b</t>
+  </si>
+  <si>
+    <t>context_core_config</t>
+  </si>
+  <si>
+    <t>context_core_status</t>
+  </si>
+  <si>
+    <t>option_core_config</t>
+  </si>
+  <si>
+    <t>option_enable_switch</t>
+  </si>
+  <si>
+    <t>option_enable_switch_always_read</t>
+  </si>
+  <si>
+    <t>option_error_normalization</t>
+  </si>
+  <si>
+    <t>option_adc_trigger_a_placement</t>
+  </si>
+  <si>
+    <t>option_adc_trigger_b_placement</t>
+  </si>
+  <si>
+    <t>option_cascade_call</t>
+  </si>
+  <si>
+    <t>data_interface_alt_input</t>
+  </si>
+  <si>
+    <t>data_interface_alt_output</t>
+  </si>
+  <si>
+    <t>data_provider_control_input</t>
+  </si>
+  <si>
+    <t>data_provider_control_error</t>
+  </si>
+  <si>
+    <t>data_provider_control_output</t>
+  </si>
+  <si>
+    <t>anti_windup_max</t>
+  </si>
+  <si>
+    <t>anti_windup_min</t>
+  </si>
+  <si>
+    <t>anti_windup_soft_desat_flag</t>
+  </si>
+  <si>
+    <t>feedback_offset_compensation</t>
+  </si>
+  <si>
+    <t>bi_directional_feedback_flag</t>
+  </si>
+  <si>
+    <t>2.0.4</t>
+  </si>
+  <si>
+    <t>04/03/2020;2.0.4;Added Token IDs for enhanced code generation option support</t>
+  </si>
+  <si>
+    <t>option_enable</t>
+  </si>
+  <si>
+    <t>data_interface_enable</t>
+  </si>
+  <si>
+    <t>data_provider_enable</t>
+  </si>
+  <si>
+    <t>anti_windup_enable</t>
+  </si>
+  <si>
+    <t>feedback_conditioning_enable</t>
+  </si>
+  <si>
+    <t>agc_enable</t>
+  </si>
+  <si>
+    <t>option_store_reload_acc</t>
+  </si>
+  <si>
+    <t>anti_windup_max_status_flag</t>
+  </si>
+  <si>
+    <t>anti_windup_min_status_flag</t>
+  </si>
+  <si>
+    <t>agc_enable_switch</t>
+  </si>
+  <si>
+    <t>agc_get_factor_function_call</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1711,6 +1804,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2031,7 +2125,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EEA387-D56E-491B-9839-D10FC585EB9A}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2090,7 +2184,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>506</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,7 +2195,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="7">
-        <v>43921</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -2119,8 +2213,8 @@
         <v>162</v>
       </c>
       <c r="C9" s="3">
-        <f>COUNTA(A10:A21)</f>
-        <v>11</v>
+        <f>COUNTA(A10:A22)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,7 +2335,18 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -2252,17 +2357,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14C6232-5B4B-4D64-8489-325A578CCED2}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -2438,7 +2545,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -2449,7 +2556,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -2460,7 +2567,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -2471,14 +2578,20 @@
         <v>342</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>164</v>
       </c>
@@ -2486,19 +2599,714 @@
         <v>162</v>
       </c>
       <c r="C22" s="3">
-        <f>COUNTA(A23:A30)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <f>COUNTA(A23:A60)</f>
+        <v>37</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="1" t="str">
+        <f>"%{(" &amp; E23 &amp; ")}%;" &amp; F23</f>
+        <v>%{(1100)}%;context_management</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="10">
+        <v>1100</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f t="shared" ref="C24:C59" si="0">"%{(" &amp; E24 &amp; ")}%;" &amp; F24</f>
+        <v>%{(1101)}%;context_shadow</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="10">
+        <v>1101</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1102)}%;context_mac_wreg</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="10">
+        <v>1102</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1103)}%;context_acc</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="10">
+        <v>1103</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1104)}%;context_acc_a</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="10">
+        <v>1104</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1105)}%;context_acc_b</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="10">
+        <v>1105</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1106)}%;context_core_config</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="10">
+        <v>1106</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>518</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1107)}%;context_core_status</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="10">
+        <v>1107</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1200)}%;option_enable</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="10">
+        <v>1200</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1201)}%;option_store_reload_acc</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="10">
+        <v>1201</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1202)}%;option_core_config</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="10">
+        <v>1202</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>11</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1203)}%;option_enable_switch</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="10">
+        <v>1203</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1204)}%;option_enable_switch_always_read</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="10">
+        <v>1204</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1205)}%;option_error_normalization</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="10">
+        <v>1205</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>14</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1206)}%;option_adc_trigger_a_placement</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="10">
+        <v>1206</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>15</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1207)}%;option_adc_trigger_b_placement</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="10">
+        <v>1207</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1208)}%;option_cascade_call</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="10">
+        <v>1208</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>17</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1209)}%;option_add_p-term</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="10">
+        <v>1209</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1300)}%;data_interface_enable</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="10">
+        <v>1300</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>19</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1301)}%;data_interface_alt_input</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="10">
+        <v>1301</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>20</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1302)}%;data_interface_alt_output</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="10">
+        <v>1302</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>21</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1400)}%;data_provider_enable</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="10">
+        <v>1400</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1401)}%;data_provider_control_input</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="10">
+        <v>1401</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>23</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1402)}%;data_provider_control_error</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="10">
+        <v>1402</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>24</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1403)}%;data_provider_control_output</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="10">
+        <v>1403</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>25</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1500)}%;anti_windup_enable</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="10">
+        <v>1500</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>26</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1501)}%;anti_windup_max</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="10">
+        <v>1501</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>27</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1502)}%;anti_windup_max_status_flag</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="10">
+        <v>1502</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>28</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1503)}%;anti_windup_min</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="10">
+        <v>1503</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>29</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1504)}%;anti_windup_min_status_flag</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="10">
+        <v>1504</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>30</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1505)}%;anti_windup_soft_desat_flag</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="10">
+        <v>1505</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>31</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1600)}%;feedback_conditioning_enable</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="10">
+        <v>1600</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>32</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1601)}%;feedback_offset_compensation</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="10">
+        <v>1601</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>33</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1602)}%;bi_directional_feedback_flag</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="10">
+        <v>1602</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>34</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1800)}%;agc_enable</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="10">
+        <v>1800</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>35</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1802)}%;agc_enable_switch</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="10">
+        <v>1802</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>36</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>%{(1803)}%;agc_get_factor_function_call</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="10">
+        <v>1803</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -4201,7 +5009,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -5496,8 +6304,9 @@
       <c r="B88" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>510</v>
+      <c r="C88" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions"</f>
+        <v>%{(1209)}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -5507,8 +6316,9 @@
       <c r="B89" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>511</v>
+      <c r="C89" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY."</f>
+        <v>%{(1209)}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY.</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -5518,8 +6328,9 @@
       <c r="B90" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>512</v>
+      <c r="C90" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS"</f>
+        <v>%{(1209)}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -5529,8 +6340,9 @@
       <c r="B91" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>513</v>
+      <c r="C91" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION"</f>
+        <v>%{(1209)}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -5540,8 +6352,9 @@
       <c r="B92" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>514</v>
+      <c r="C92" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)"</f>
+        <v>%{(1209)}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -5551,8 +6364,9 @@
       <c r="B93" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>515</v>
+      <c r="C93" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object"</f>
+        <v>%{(1209)}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -5562,8 +6376,9 @@
       <c r="B94" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>516</v>
+      <c r="C94" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%);"</f>
+        <v>%{(1209)}%%IDENT%);</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -5573,8 +6388,9 @@
       <c r="B95" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>517</v>
+      <c r="C95" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%EMPTY%"</f>
+        <v>%{(1209)}%%EMPTY%</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6607,7 +7423,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated source code generator script Excel sheets
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F72C68-6AD5-435D-8B85-3EF918AE5AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A3D7E1-BE3D-42F8-9DE3-7E8232B16F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="7" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="5" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="557">
   <si>
     <t>line0</t>
   </si>
@@ -1690,6 +1690,27 @@
   </si>
   <si>
     <t>agc_get_factor_function_call</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%// P-Term Coefficients (for plant measurements only)</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile int16_t PTermFactor; // Q15 P-Term Coefficient Factor (R/W)</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile int16_t PTermScaler; // Q15 P-Term Coefficient Bit-Shift Scaler (R/W)</t>
+  </si>
+  <si>
+    <t>line174</t>
+  </si>
+  <si>
+    <t>line175</t>
+  </si>
+  <si>
+    <t>line176</t>
+  </si>
+  <si>
+    <t>line177</t>
   </si>
 </sst>
 </file>
@@ -3376,9 +3397,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798E1EF1-7DA6-47D5-9A26-6753C89CA0C2}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3403,7 +3426,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4712,7 +4735,7 @@
         <v>162</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>421</v>
+        <v>173</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -4723,7 +4746,7 @@
         <v>162</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>173</v>
+        <v>550</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -4734,7 +4757,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>502</v>
+        <v>552</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4745,7 +4768,7 @@
         <v>162</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>191</v>
+        <v>551</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4756,7 +4779,7 @@
         <v>162</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -4767,7 +4790,7 @@
         <v>162</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>411</v>
+        <v>173</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -4778,7 +4801,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>492</v>
+        <v>502</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -4789,7 +4812,7 @@
         <v>162</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>493</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -4800,7 +4823,7 @@
         <v>162</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -4811,7 +4834,7 @@
         <v>162</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>173</v>
+        <v>411</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -4822,7 +4845,7 @@
         <v>162</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>211</v>
+        <v>492</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4833,7 +4856,7 @@
         <v>162</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>191</v>
+        <v>493</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4867,7 @@
         <v>162</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -4855,7 +4878,7 @@
         <v>162</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>413</v>
+        <v>173</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -4866,7 +4889,7 @@
         <v>162</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>414</v>
+        <v>211</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -4877,7 +4900,7 @@
         <v>162</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>415</v>
+        <v>191</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -4888,7 +4911,7 @@
         <v>162</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>503</v>
+        <v>412</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -4899,7 +4922,7 @@
         <v>162</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>173</v>
+        <v>413</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -4910,7 +4933,7 @@
         <v>162</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -4921,7 +4944,7 @@
         <v>162</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>191</v>
+        <v>415</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -4932,7 +4955,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4943,7 +4966,7 @@
         <v>162</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>490</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -4954,7 +4977,7 @@
         <v>162</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>491</v>
+        <v>212</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -4965,7 +4988,7 @@
         <v>162</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>419</v>
+        <v>191</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4976,7 +4999,7 @@
         <v>162</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>173</v>
+        <v>489</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -4987,7 +5010,7 @@
         <v>162</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>417</v>
+        <v>490</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -4998,7 +5021,7 @@
         <v>162</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>191</v>
+        <v>491</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -5009,7 +5032,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>507</v>
+        <v>419</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -5020,7 +5043,7 @@
         <v>162</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>416</v>
+        <v>173</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -5031,7 +5054,7 @@
         <v>162</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -5042,7 +5065,7 @@
         <v>162</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -5053,7 +5076,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>488</v>
+        <v>507</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -5064,7 +5087,7 @@
         <v>162</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>191</v>
+        <v>416</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -5075,7 +5098,7 @@
         <v>162</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>474</v>
+        <v>418</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -5086,7 +5109,7 @@
         <v>162</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>475</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -5097,7 +5120,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>476</v>
+        <v>488</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -5108,7 +5131,7 @@
         <v>162</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>477</v>
+        <v>191</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -5119,7 +5142,7 @@
         <v>162</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>173</v>
+        <v>474</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -5130,7 +5153,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -5141,7 +5164,7 @@
         <v>162</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>191</v>
+        <v>476</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -5152,7 +5175,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -5163,7 +5186,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>480</v>
+        <v>173</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -5174,7 +5197,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -5185,7 +5208,7 @@
         <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>482</v>
+        <v>191</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -5196,7 +5219,7 @@
         <v>162</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>441</v>
+        <v>479</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -5207,7 +5230,7 @@
         <v>162</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>173</v>
+        <v>480</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -5218,7 +5241,7 @@
         <v>162</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>213</v>
+        <v>481</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -5229,7 +5252,7 @@
         <v>162</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>173</v>
+        <v>482</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -5240,7 +5263,7 @@
         <v>162</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -5251,7 +5274,7 @@
         <v>162</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>440</v>
+        <v>173</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -5262,7 +5285,7 @@
         <v>162</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -5284,7 +5307,7 @@
         <v>162</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>214</v>
+        <v>439</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -5295,7 +5318,7 @@
         <v>162</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>215</v>
+        <v>440</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -5306,7 +5329,7 @@
         <v>162</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -5317,6 +5340,50 @@
         <v>162</v>
       </c>
       <c r="C176" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C180" s="2" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5332,8 +5399,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6491,9 +6558,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA645C0-6722-49C9-83B9-8B808C24A9CC}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6518,7 +6587,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -7315,8 +7384,9 @@
       <c r="B74" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>173</v>
+      <c r="C74" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%EMPTY%"</f>
+        <v>%{(1209)}%%EMPTY%</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -7326,8 +7396,9 @@
       <c r="B75" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>272</v>
+      <c r="C75" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// P-Term Coefficient for Plant Measurements"</f>
+        <v>%{(1209)}%// P-Term Coefficient for Plant Measurements</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -7337,8 +7408,9 @@
       <c r="B76" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>173</v>
+      <c r="C76" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%volatile int16_t %PREFIX%pterm_factor = %PTERMFACTOR%;"</f>
+        <v>%{(1209)}%volatile int16_t %PREFIX%pterm_factor = %PTERMFACTOR%;</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -7348,8 +7420,9 @@
       <c r="B77" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>271</v>
+      <c r="C77" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%volatile int16_t %PREFIX%pterm_scaler = %PTERMSCALER%;"</f>
+        <v>%{(1209)}%volatile int16_t %PREFIX%pterm_scaler = %PTERMSCALER%;</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -7360,6 +7433,50 @@
         <v>162</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>173</v>
       </c>
     </row>
@@ -7421,10 +7538,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3AE5A0-DD2C-4692-866D-4B2E06E8D02C}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7450,7 +7567,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8098,8 +8215,9 @@
       <c r="B61" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>304</v>
+      <c r="C61" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%"</f>
+        <v>%{(1209)}%%IDENT%</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -8109,8 +8227,9 @@
       <c r="B62" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>303</v>
+      <c r="C62" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%// Load P-Term factor and scaler into data structure"</f>
+        <v>%{(1209)}%%IDENT%// Load P-Term factor and scaler into data structure</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -8120,8 +8239,9 @@
       <c r="B63" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>302</v>
+      <c r="C63" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%controller-&gt;Filter.PTermFactor = %PREFIX%pterm_factor;;"</f>
+        <v>%{(1209)}%%IDENT%controller-&gt;Filter.PTermFactor = %PREFIX%pterm_factor;;</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -8131,8 +8251,9 @@
       <c r="B64" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>173</v>
+      <c r="C64" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%controller-&gt;Filter.PTermScaler = %PREFIX%pterm_scaler;"</f>
+        <v>%{(1209)}%%IDENT%controller-&gt;Filter.PTermScaler = %PREFIX%pterm_scaler;</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -8143,7 +8264,7 @@
         <v>162</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>173</v>
+        <v>304</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -8154,7 +8275,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>214</v>
+        <v>303</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -8165,7 +8286,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>215</v>
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -8176,7 +8297,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -8187,6 +8308,50 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Applied new option tokens to all control loop types from SBSFT to FSCL During the process the execution list was reviewed and harmonized. All control loops now apply the same execution list with the exception of their individual scaling instruction sets.
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70837C30-27EB-43AC-9571-4D7A21A7BCB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC1FB8-330B-4373-A1E6-F0B13C8FC87F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="5" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="1" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -2380,8 +2380,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,11 +3301,11 @@
       </c>
       <c r="C58" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>%{(1802)}%;agc_enable_switch</v>
+        <v>%{(1801)}%;agc_enable_switch</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="10">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>548</v>
@@ -3320,11 +3320,11 @@
       </c>
       <c r="C59" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>%{(1803)}%;agc_get_factor_function_call</v>
+        <v>%{(1802)}%;agc_get_factor_function_call</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="10">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>549</v>
@@ -6560,7 +6560,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added info text on used resources to Context Management box
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC1FB8-330B-4373-A1E6-F0B13C8FC87F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD962B43-AF00-4C69-84A7-2546A4DED8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="1" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="3" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -1308,9 +1308,6 @@
     <t>%IDENT%} __attribute__((packed))Filter; // Filter parameters such as pointer to history and coefficient arrays and number scaling</t>
   </si>
   <si>
-    <t>%IDENT%volatile CONTROLLER_STATUS_t status; // Control Loop Status and Control flags</t>
-  </si>
-  <si>
     <t xml:space="preserve">%IDENT%%IDENT%volatile int32_t* ptrACoefficients; // Pointer to A coefficients located in X-space </t>
   </si>
   <si>
@@ -1711,6 +1708,9 @@
   </si>
   <si>
     <t>line177</t>
+  </si>
+  <si>
+    <t>%IDENT%volatile CONTROLLER_STATUS_t Status; // Control Loop Status and Control flags</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2183,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2205,7 +2205,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2268,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2312,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -2380,7 +2380,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:B59"/>
     </sheetView>
   </sheetViews>
@@ -2541,7 +2541,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2601,15 +2601,15 @@
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>509</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2643,7 +2643,7 @@
         <v>1100</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>1101</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2681,7 +2681,7 @@
         <v>1102</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2700,7 +2700,7 @@
         <v>1103</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>1104</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
         <v>1105</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>1106</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2776,7 +2776,7 @@
         <v>1107</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,7 +2795,7 @@
         <v>1200</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>1201</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2833,7 +2833,7 @@
         <v>1202</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2852,7 +2852,7 @@
         <v>1203</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
         <v>1204</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
         <v>1205</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2909,7 +2909,7 @@
         <v>1206</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>1207</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2947,7 +2947,7 @@
         <v>1208</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,7 +2966,7 @@
         <v>1209</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,7 +2985,7 @@
         <v>1300</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,7 +3004,7 @@
         <v>1301</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
         <v>1302</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,7 +3042,7 @@
         <v>1400</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
         <v>1401</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>1402</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>1403</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3118,7 +3118,7 @@
         <v>1500</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
         <v>1501</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3156,7 +3156,7 @@
         <v>1502</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3175,7 +3175,7 @@
         <v>1503</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3194,7 +3194,7 @@
         <v>1504</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3213,7 +3213,7 @@
         <v>1505</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>1600</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
         <v>1601</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -3270,7 +3270,7 @@
         <v>1602</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -3289,7 +3289,7 @@
         <v>1800</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -3308,7 +3308,7 @@
         <v>1801</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
         <v>1802</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -3399,8 +3399,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C180"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="B76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3492,7 +3492,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3602,7 +3602,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3624,7 +3624,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3635,7 +3635,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3646,7 +3646,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3657,7 +3657,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3734,7 +3734,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3943,7 +3943,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3954,7 +3954,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4218,7 +4218,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4262,7 +4262,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -4328,7 +4328,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -4339,7 +4339,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -4350,7 +4350,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -4361,7 +4361,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -4372,7 +4372,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>422</v>
+        <v>556</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -4460,7 +4460,7 @@
         <v>162</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -4471,7 +4471,7 @@
         <v>162</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -4482,7 +4482,7 @@
         <v>162</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -4493,7 +4493,7 @@
         <v>162</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -4515,7 +4515,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -4559,7 +4559,7 @@
         <v>162</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -4570,7 +4570,7 @@
         <v>162</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>162</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -4757,7 +4757,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4768,7 +4768,7 @@
         <v>162</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4801,7 +4801,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -4845,7 +4845,7 @@
         <v>162</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4856,7 +4856,7 @@
         <v>162</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -4955,7 +4955,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4999,7 +4999,7 @@
         <v>162</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -5010,7 +5010,7 @@
         <v>162</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -5021,7 +5021,7 @@
         <v>162</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -5076,7 +5076,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -5120,7 +5120,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -5142,7 +5142,7 @@
         <v>162</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -5153,7 +5153,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -5164,7 +5164,7 @@
         <v>162</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -5175,7 +5175,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -5197,7 +5197,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -5213,62 +5213,62 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>162</v>
@@ -5279,7 +5279,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>162</v>
@@ -5290,7 +5290,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>162</v>
@@ -5301,29 +5301,29 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>162</v>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>162</v>
@@ -5345,7 +5345,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>162</v>
@@ -5356,7 +5356,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>162</v>
@@ -5367,7 +5367,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>162</v>
@@ -5378,7 +5378,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>162</v>
@@ -5602,7 +5602,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6317,7 +6317,7 @@
         <v>162</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6763,7 +6763,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -7897,7 +7897,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -7908,7 +7908,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -7919,7 +7919,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -7930,7 +7930,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -7941,7 +7941,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -7952,7 +7952,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -7963,7 +7963,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -7974,7 +7974,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -7996,7 +7996,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -8007,7 +8007,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -8018,7 +8018,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -8029,7 +8029,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -8073,7 +8073,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -8139,7 +8139,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code generator script generators
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD962B43-AF00-4C69-84A7-2546A4DED8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BDEFFF-9AA4-41F0-8324-075C722976D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="3" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="561">
   <si>
     <t>line0</t>
   </si>
@@ -1461,15 +1461,6 @@
     <t>%IDENT%%IDENT%volatile CONTROLLER_PORT_t AltTarget; // Secondary data output port declaration</t>
   </si>
   <si>
-    <t>%IDENT%%IDENT%volatile uint16_t agcScaler; // Bit-shift scaler of Adaptive Gain Modulation factor</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile fractional agcFactor; // Q15 value of Adaptive Gain Modulation factor</t>
-  </si>
-  <si>
-    <t>%IDENT%%IDENT%volatile fractional agcMedian; // Q15 value of Adaptive Gain Modulation nominal operating point</t>
-  </si>
-  <si>
     <t>%IDENT%} __attribute__((packed))GainControl; // Parameter section for advanced control options</t>
   </si>
   <si>
@@ -1650,9 +1641,6 @@
     <t>bi_directional_feedback_flag</t>
   </si>
   <si>
-    <t>2.0.4</t>
-  </si>
-  <si>
     <t>04/03/2020;2.0.4;Added Token IDs for enhanced code generation option support</t>
   </si>
   <si>
@@ -1710,7 +1698,31 @@
     <t>line177</t>
   </si>
   <si>
-    <t>%IDENT%volatile CONTROLLER_STATUS_t Status; // Control Loop Status and Control flags</t>
+    <t>// User-defined cNPNZ_t controller data object</t>
+  </si>
+  <si>
+    <t>line178</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t* ptrAgcObserverFunction; // Function Pointer to Observer function updating the AGC modulation factor</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile uint16_t AgcScaler; // Bit-shift scaler of Adaptive Gain Modulation factor</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile fractional AgcFactor; // Q15 value of Adaptive Gain Modulation factor</t>
+  </si>
+  <si>
+    <t>%IDENT%%IDENT%volatile fractional AgcMedian; // Q15 value of Adaptive Gain Modulation nominal operating point</t>
+  </si>
+  <si>
+    <t>2.0.5</t>
+  </si>
+  <si>
+    <t>04/21/2020;2.0.5;Added user-defined function pointer to observer function to AGC declarations</t>
+  </si>
+  <si>
+    <t>%IDENT%volatile CONTROLLER_STATUS_t status; // Control Loop Status and Control flags</t>
   </si>
 </sst>
 </file>
@@ -2146,7 +2158,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EEA387-D56E-491B-9839-D10FC585EB9A}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2205,7 +2217,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>536</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2216,7 +2228,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="7">
-        <v>43924</v>
+        <v>43942</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -2234,8 +2246,8 @@
         <v>162</v>
       </c>
       <c r="C9" s="3">
-        <f>COUNTA(A10:A22)</f>
-        <v>12</v>
+        <f>COUNTA(A10:A23)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2346,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2357,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,7 +2368,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2379,18 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>537</v>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -2380,8 +2403,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:B59"/>
+    <sheetView topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,15 +2624,15 @@
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" s="5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2643,7 +2666,7 @@
         <v>1100</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2662,7 +2685,7 @@
         <v>1101</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2681,7 +2704,7 @@
         <v>1102</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2700,7 +2723,7 @@
         <v>1103</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2719,7 +2742,7 @@
         <v>1104</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2738,7 +2761,7 @@
         <v>1105</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2757,7 +2780,7 @@
         <v>1106</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2776,7 +2799,7 @@
         <v>1107</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,7 +2818,7 @@
         <v>1200</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2814,7 +2837,7 @@
         <v>1201</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2833,7 +2856,7 @@
         <v>1202</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2852,7 +2875,7 @@
         <v>1203</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,7 +2894,7 @@
         <v>1204</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2890,7 +2913,7 @@
         <v>1205</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2909,7 +2932,7 @@
         <v>1206</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2928,7 +2951,7 @@
         <v>1207</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2947,7 +2970,7 @@
         <v>1208</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,7 +2989,7 @@
         <v>1209</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,7 +3008,7 @@
         <v>1300</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,7 +3027,7 @@
         <v>1301</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3023,7 +3046,7 @@
         <v>1302</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,7 +3065,7 @@
         <v>1400</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3061,7 +3084,7 @@
         <v>1401</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,7 +3103,7 @@
         <v>1402</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3099,7 +3122,7 @@
         <v>1403</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3118,7 +3141,7 @@
         <v>1500</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3137,7 +3160,7 @@
         <v>1501</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3156,7 +3179,7 @@
         <v>1502</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3175,7 +3198,7 @@
         <v>1503</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3194,7 +3217,7 @@
         <v>1504</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3213,7 +3236,7 @@
         <v>1505</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,7 +3255,7 @@
         <v>1600</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3251,7 +3274,7 @@
         <v>1601</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -3270,7 +3293,7 @@
         <v>1602</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -3289,7 +3312,7 @@
         <v>1800</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -3308,7 +3331,7 @@
         <v>1801</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3327,7 +3350,7 @@
         <v>1802</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -3397,7 +3420,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798E1EF1-7DA6-47D5-9A26-6753C89CA0C2}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C93" sqref="C93"/>
@@ -3426,7 +3449,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3954,7 +3977,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4218,7 +4241,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4328,7 +4351,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -4339,7 +4362,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -4350,7 +4373,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -4361,7 +4384,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -4416,7 +4439,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -4515,7 +4538,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -4746,7 +4769,7 @@
         <v>162</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -4757,7 +4780,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4768,7 +4791,7 @@
         <v>162</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4801,7 +4824,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -4845,7 +4868,7 @@
         <v>162</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4856,7 +4879,7 @@
         <v>162</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -4955,7 +4978,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4999,7 +5022,7 @@
         <v>162</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -5010,7 +5033,7 @@
         <v>162</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -5021,7 +5044,7 @@
         <v>162</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -5076,7 +5099,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -5120,7 +5143,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -5142,7 +5165,7 @@
         <v>162</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>473</v>
+        <v>555</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -5153,7 +5176,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>474</v>
+        <v>556</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -5164,7 +5187,7 @@
         <v>162</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>475</v>
+        <v>557</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -5175,7 +5198,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>476</v>
+        <v>554</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -5186,7 +5209,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>173</v>
+        <v>473</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -5197,7 +5220,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>477</v>
+        <v>173</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -5208,7 +5231,7 @@
         <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>191</v>
+        <v>474</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -5219,7 +5242,7 @@
         <v>162</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>478</v>
+        <v>191</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -5230,7 +5253,7 @@
         <v>162</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -5241,7 +5264,7 @@
         <v>162</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -5252,7 +5275,7 @@
         <v>162</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -5263,7 +5286,7 @@
         <v>162</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>440</v>
+        <v>478</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -5274,7 +5297,7 @@
         <v>162</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>173</v>
+        <v>440</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -5285,56 +5308,56 @@
         <v>162</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>438</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>173</v>
+        <v>439</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>162</v>
@@ -5345,45 +5368,56 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C180" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C181" s="2" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5397,10 +5431,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C06CF0-653A-4427-B7AE-138E1BDF5DAA}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5426,7 +5460,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6041,8 +6075,9 @@
       <c r="B58" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>173</v>
+      <c r="C58" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%%EMPTY%"</f>
+        <v>%{(1209)}%%EMPTY%</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6052,8 +6087,9 @@
       <c r="B59" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>173</v>
+      <c r="C59" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%// P-Term Coefficient for Plant Measurements"</f>
+        <v>%{(1209)}%// P-Term Coefficient for Plant Measurements</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6063,8 +6099,9 @@
       <c r="B60" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>257</v>
+      <c r="C60" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%extern volatile int16_t %PREFIX%pterm_factor;"</f>
+        <v>%{(1209)}%extern volatile int16_t %PREFIX%pterm_factor;</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6074,8 +6111,9 @@
       <c r="B61" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>173</v>
+      <c r="C61" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%extern volatile int16_t %PREFIX%pterm_scaler;"</f>
+        <v>%{(1209)}%extern volatile int16_t %PREFIX%pterm_scaler;</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6085,8 +6123,9 @@
       <c r="B62" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>237</v>
+      <c r="C62" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%%EMPTY%"</f>
+        <v>%{(1800)}%%EMPTY%</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6096,8 +6135,9 @@
       <c r="B63" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>258</v>
+      <c r="C63" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%//Adaptive Gain Control Coefficient"</f>
+        <v>%{(1800)}%//Adaptive Gain Control Coefficient</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -6107,8 +6147,9 @@
       <c r="B64" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>248</v>
+      <c r="C64" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%extern volatile int16_t %PREFIX%agc_factor_default;"</f>
+        <v>%{(1800)}%extern volatile int16_t %PREFIX%agc_factor_default;</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6118,8 +6159,9 @@
       <c r="B65" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>173</v>
+      <c r="C65" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%extern volatile int16_t %PREFIX%agc_scaler_default;"</f>
+        <v>%{(1800)}%extern volatile int16_t %PREFIX%agc_scaler_default;</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6130,7 +6172,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>259</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6141,7 +6183,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>395</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6152,7 +6194,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>260</v>
+        <v>552</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6163,7 +6205,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6185,7 +6227,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6196,7 +6238,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6207,7 +6249,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6218,7 +6260,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>261</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6229,7 +6271,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>173</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6240,7 +6282,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>264</v>
+        <v>395</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6251,7 +6293,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6262,7 +6304,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6273,7 +6315,7 @@
         <v>162</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>267</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -6284,7 +6326,7 @@
         <v>162</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6295,7 +6337,7 @@
         <v>162</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6306,7 +6348,7 @@
         <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>173</v>
+        <v>260</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -6317,7 +6359,7 @@
         <v>162</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>504</v>
+        <v>261</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6328,7 +6370,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>269</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -6339,7 +6381,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6350,7 +6392,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6361,7 +6403,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>173</v>
+        <v>266</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6371,9 +6413,8 @@
       <c r="B88" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C88" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions"</f>
-        <v>%{(1209)}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions</v>
+      <c r="C88" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -6383,9 +6424,8 @@
       <c r="B89" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C89" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY."</f>
-        <v>%{(1209)}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY.</v>
+      <c r="C89" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6395,9 +6435,8 @@
       <c r="B90" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C90" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS"</f>
-        <v>%{(1209)}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS</v>
+      <c r="C90" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6407,9 +6446,8 @@
       <c r="B91" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C91" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION"</f>
-        <v>%{(1209)}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION</v>
+      <c r="C91" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -6419,9 +6457,8 @@
       <c r="B92" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C92" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)"</f>
-        <v>%{(1209)}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)</v>
+      <c r="C92" s="1" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6431,9 +6468,8 @@
       <c r="B93" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C93" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object"</f>
-        <v>%{(1209)}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object</v>
+      <c r="C93" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6443,9 +6479,8 @@
       <c r="B94" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C94" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%IDENT%);"</f>
-        <v>%{(1209)}%%IDENT%);</v>
+      <c r="C94" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6455,9 +6490,8 @@
       <c r="B95" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C95" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%EMPTY%"</f>
-        <v>%{(1209)}%%EMPTY%</v>
+      <c r="C95" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6478,8 +6512,9 @@
       <c r="B97" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>270</v>
+      <c r="C97" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions"</f>
+        <v>%{(1209)}%// Calls the %FILENAME_PATTERN% P-Term controller during measurements of plant transfer functions</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6489,8 +6524,9 @@
       <c r="B98" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>173</v>
+      <c r="C98" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY."</f>
+        <v>%{(1209)}%// THIS CONTROLLER IS USED FOR MEASUREMENTS OF THE PLANT TRANSFER FUNCTION ONLY.</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6500,8 +6536,9 @@
       <c r="B99" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>173</v>
+      <c r="C99" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS"</f>
+        <v>%{(1209)}%// THIS LOOP IS BY DEFAULT UNSTABLE AND ONLY WORKS UNDER STABLE TEST CONDITIONS</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6511,8 +6548,9 @@
       <c r="B100" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>214</v>
+      <c r="C100" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION"</f>
+        <v>%{(1209)}%// DO NOT USE THIS CONTROLLER TYPE FOR NORMAL OPERATION</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6522,8 +6560,9 @@
       <c r="B101" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>215</v>
+      <c r="C101" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)"</f>
+        <v>%{(1209)}%extern void %FILENAME_PATTERN%_PTermUpdate( // Calls the P-Term controller (Assembly)</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -6533,8 +6572,9 @@
       <c r="B102" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>214</v>
+      <c r="C102" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object"</f>
+        <v>%{(1209)}%%IDENT%%IDENT%volatile %STRUCTURE_LABEL%* controller // Pointer to nPnZ data type object</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6544,7 +6584,108 @@
       <c r="B103" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%%IDENT%);"</f>
+        <v>%{(1209)}%%IDENT%);</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C104" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%%EMPTY%"</f>
+        <v>%{(1209)}%%EMPTY%</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>173</v>
       </c>
     </row>
@@ -6558,10 +6699,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA645C0-6722-49C9-83B9-8B808C24A9CC}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6587,7 +6728,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -7385,7 +7526,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%%EMPTY%"</f>
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%%EMPTY%"</f>
         <v>%{(1209)}%%EMPTY%</v>
       </c>
     </row>
@@ -7397,7 +7538,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%// P-Term Coefficient for Plant Measurements"</f>
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%// P-Term Coefficient for Plant Measurements"</f>
         <v>%{(1209)}%// P-Term Coefficient for Plant Measurements</v>
       </c>
     </row>
@@ -7409,7 +7550,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%volatile int16_t %PREFIX%pterm_factor = %PTERMFACTOR%;"</f>
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%volatile int16_t %PREFIX%pterm_factor = %PTERMFACTOR%;"</f>
         <v>%{(1209)}%volatile int16_t %PREFIX%pterm_factor = %PTERMFACTOR%;</v>
       </c>
     </row>
@@ -7421,7 +7562,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="1" t="str">
-        <f xml:space="preserve"> "%{(" &amp; tokens!E40 &amp; ")}%volatile int16_t %PREFIX%pterm_scaler = %PTERMSCALER%;"</f>
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$40 &amp; ")}%volatile int16_t %PREFIX%pterm_scaler = %PTERMSCALER%;"</f>
         <v>%{(1209)}%volatile int16_t %PREFIX%pterm_scaler = %PTERMSCALER%;</v>
       </c>
     </row>
@@ -7432,8 +7573,9 @@
       <c r="B78" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>173</v>
+      <c r="C78" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%%EMPTY%"</f>
+        <v>%{(1800)}%%EMPTY%</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -7443,8 +7585,9 @@
       <c r="B79" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>272</v>
+      <c r="C79" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%//Adaptive Gain Control Coefficient"</f>
+        <v>%{(1800)}%//Adaptive Gain Control Coefficient</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -7454,8 +7597,9 @@
       <c r="B80" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>173</v>
+      <c r="C80" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%volatile int16_t %PREFIX%agc_factor_default = %AGCFACTOR%;"</f>
+        <v>%{(1800)}%volatile int16_t %PREFIX%agc_factor_default = %AGCFACTOR%;</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -7465,8 +7609,9 @@
       <c r="B81" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>271</v>
+      <c r="C81" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!$E$57 &amp; ")}%volatile int16_t %PREFIX%agc_scaler_default = %AGCSCALER%;"</f>
+        <v>%{(1800)}%volatile int16_t %PREFIX%agc_scaler_default = %AGCSCALER%;</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -7477,6 +7622,72 @@
         <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>173</v>
       </c>
     </row>
@@ -7538,10 +7749,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3AE5A0-DD2C-4692-866D-4B2E06E8D02C}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7567,7 +7778,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTA(A:A)-2</f>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8263,8 +8474,9 @@
       <c r="B65" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>304</v>
+      <c r="C65" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E$57 &amp; ")}%%IDENT%"</f>
+        <v>%{(1800)}%%IDENT%</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -8274,8 +8486,9 @@
       <c r="B66" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>303</v>
+      <c r="C66" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E$57 &amp; ")}%%IDENT%// Load initial AGC factor and scaler into data structure"</f>
+        <v>%{(1800)}%%IDENT%// Load initial AGC factor and scaler into data structure</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -8285,8 +8498,9 @@
       <c r="B67" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>302</v>
+      <c r="C67" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E$57 &amp; ")}%%IDENT%controller-&gt;GainControl.AgcFactor = %PREFIX%agc_factor_default;"</f>
+        <v>%{(1800)}%%IDENT%controller-&gt;GainControl.AgcFactor = %PREFIX%agc_factor_default;</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -8296,8 +8510,9 @@
       <c r="B68" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>173</v>
+      <c r="C68" s="1" t="str">
+        <f xml:space="preserve"> "%{(" &amp; tokens!E$57 &amp; ")}%%IDENT%controller-&gt;GainControl.AgcScaler = %PREFIX%agc_scaler_default;"</f>
+        <v>%{(1800)}%%IDENT%controller-&gt;GainControl.AgcScaler = %PREFIX%agc_scaler_default;</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -8308,7 +8523,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>173</v>
+        <v>304</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -8319,7 +8534,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>214</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -8330,7 +8545,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>215</v>
+        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -8341,7 +8556,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -8352,6 +8567,50 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated C-Code generator script generator file
</commit_message>
<xml_diff>
--- a/tools/c-gen_builder.xlsx
+++ b/tools/c-gen_builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Digital Control Library SDK\WindowsForms\Digital Control Loop Designer zDLD\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BDEFFF-9AA4-41F0-8324-075C722976D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE334AA3-6F3A-4A48-9153-2D9FA9A14E0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="3" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="654" activeTab="7" xr2:uid="{69E5396C-D40F-4CA2-80D3-E50D1E02D17F}"/>
   </bookViews>
   <sheets>
     <sheet name="PreText" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="551">
   <si>
     <t>line0</t>
   </si>
@@ -537,24 +537,6 @@
     <t>count</t>
   </si>
   <si>
-    <t>/* ********************************************************************************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * %APP_PRODUCT_NAME%, Version %APP_PRODUCT_VERSION%</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * ********************************************************************************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * Generic library header for z-domain compensation filter assembly functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * CGS Version: %CGS_VERSION%</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * ********************************************************************************/</t>
-  </si>
-  <si>
     <t>#ifndef __SPECIAL_FUNCTION_LAYER_LIB_NPNZ_H__</t>
   </si>
   <si>
@@ -702,9 +684,6 @@
     <t>%SPACE%* %APP_PRODUCT_NAME%, Version %APP_PRODUCT_VERSION%</t>
   </si>
   <si>
-    <t>%SPACE%* ********************************************************************************</t>
-  </si>
-  <si>
     <t>%SPACE%* %FILTER_ORDER%p%FILTER_ORDER%z controller function declarations and compensation filter coefficients</t>
   </si>
   <si>
@@ -729,9 +708,6 @@
     <t>%SPACE%*  Input Gain:         %INPUT_GAIN%</t>
   </si>
   <si>
-    <t>%SPACE%* *******************************************************************************</t>
-  </si>
-  <si>
     <t>%SPACE%* CGS Version:         %CGS_VERSION%</t>
   </si>
   <si>
@@ -741,9 +717,6 @@
     <t>%SPACE%* Date/Time:           %DATE_TODAY%</t>
   </si>
   <si>
-    <t>%SPACE%* *******************************************************************************/</t>
-  </si>
-  <si>
     <t>#ifndef __SPECIAL_FUNCTION_LAYER_%FILENAME_PATTERN_U%_H__</t>
   </si>
   <si>
@@ -900,9 +873,6 @@
     <t xml:space="preserve">volatile %PREFIXU%CONTROL_LOOP_COEFFICIENTS_t __attribute__((space(xmemory), near)) %PREFIX%coefficients; // A/B-Coefficients </t>
   </si>
   <si>
-    <t>%SPACE%* through defines in source file %FILENAME_PATTERN_L%.c</t>
-  </si>
-  <si>
     <t xml:space="preserve">%SPACE%* length and memory location. These declarations are made publicly accessible </t>
   </si>
   <si>
@@ -930,18 +900,6 @@
     <t>#include "%C_HEADER_INCLUDE_PATH%"</t>
   </si>
   <si>
-    <t>%SPACE%* **********************************************************************************</t>
-  </si>
-  <si>
-    <t>%SPACE%* conditions:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%SPACE%* %FILTER_ORDER%p%FILTER_ORDER%z compensation filter coefficients derived for following operating </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      /* **********************************************************************************</t>
-  </si>
-  <si>
     <t>[comp_source_head]</t>
   </si>
   <si>
@@ -1380,9 +1338,6 @@
     <t>// This version key represents the product version of DCLD as integer number</t>
   </si>
   <si>
-    <t>// of the form [MAJOR][MINOR][REVISION] =&gt; version 0.9.03 would be shown as 903</t>
-  </si>
-  <si>
     <t>#ifndef __DCLD_VERSION</t>
   </si>
   <si>
@@ -1395,18 +1350,12 @@
     <t>%CGS_VERSION_DATE%</t>
   </si>
   <si>
-    <t xml:space="preserve"> * CGS Date:    %CGS_VERSION_DATE%</t>
-  </si>
-  <si>
     <t>%SPACE%* CGS Date:            %CGS_VERSION_DATE%</t>
   </si>
   <si>
     <t>03/25/2020;1.1.5;Fixed typo in CGS_VERSION_DATE token</t>
   </si>
   <si>
-    <t>%IDENT%#define __DCLD_VERSION    903</t>
-  </si>
-  <si>
     <t>#endif  // end of __DCLD_VERSION</t>
   </si>
   <si>
@@ -1716,13 +1665,34 @@
     <t>%IDENT%%IDENT%volatile fractional AgcMedian; // Q15 value of Adaptive Gain Modulation nominal operating point</t>
   </si>
   <si>
-    <t>2.0.5</t>
-  </si>
-  <si>
     <t>04/21/2020;2.0.5;Added user-defined function pointer to observer function to AGC declarations</t>
   </si>
   <si>
     <t>%IDENT%volatile CONTROLLER_STATUS_t status; // Control Loop Status and Control flags</t>
+  </si>
+  <si>
+    <t>%SPACE%* through extern declarations in header file %FILENAME_PATTERN_L%.h</t>
+  </si>
+  <si>
+    <t>%IDENT%#define __DCLD_VERSION    %DCLD_VERSION_CODE%</t>
+  </si>
+  <si>
+    <t>// of the form [MAJOR][MINOR][REVISION] =&gt; version 0.9.3.xxx would be shown as 903</t>
+  </si>
+  <si>
+    <t>2.0.6</t>
+  </si>
+  <si>
+    <t>04/23/2020;2.0.6;Fixed comments in C-Source file and bug not updating DCD version code</t>
+  </si>
+  <si>
+    <t>%SPACE%* Generic library header for z-domain compensation filter assembly functions</t>
+  </si>
+  <si>
+    <t>%SPACE%* CGS Version: %CGS_VERSION%</t>
+  </si>
+  <si>
+    <t>%SPACE%* CGS Date:    %CGS_VERSION_DATE%</t>
   </si>
 </sst>
 </file>
@@ -2158,7 +2128,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EEA387-D56E-491B-9839-D10FC585EB9A}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2171,69 +2141,69 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>558</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C6" s="7">
-        <v>43942</v>
+        <v>43944</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2246,8 +2216,8 @@
         <v>162</v>
       </c>
       <c r="C9" s="3">
-        <f>COUNTA(A10:A23)</f>
-        <v>13</v>
+        <f>COUNTA(A10:A24)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2258,7 +2228,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2269,7 +2239,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2280,7 +2250,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2291,7 +2261,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2302,7 +2272,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2313,7 +2283,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2324,7 +2294,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2335,7 +2305,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2346,7 +2316,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2357,7 +2327,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2368,7 +2338,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,7 +2349,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2390,7 +2360,18 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>559</v>
+        <v>541</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -2418,7 +2399,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2443,7 +2424,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2454,7 +2435,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,7 +2446,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2476,7 +2457,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2487,7 +2468,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2498,7 +2479,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2509,7 +2490,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2520,7 +2501,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2531,7 +2512,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2542,7 +2523,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2553,7 +2534,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2564,7 +2545,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2575,7 +2556,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2586,7 +2567,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2597,7 +2578,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2608,7 +2589,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2619,20 +2600,20 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" s="5" t="s">
-        <v>505</v>
+        <v>488</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2666,7 +2647,7 @@
         <v>1100</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>507</v>
+        <v>490</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2685,7 +2666,7 @@
         <v>1101</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>509</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2704,7 +2685,7 @@
         <v>1102</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>510</v>
+        <v>493</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2723,7 +2704,7 @@
         <v>1103</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>511</v>
+        <v>494</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2742,7 +2723,7 @@
         <v>1104</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2761,7 +2742,7 @@
         <v>1105</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2780,7 +2761,7 @@
         <v>1106</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2799,7 +2780,7 @@
         <v>1107</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2818,7 +2799,7 @@
         <v>1200</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>534</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2837,7 +2818,7 @@
         <v>1201</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2856,7 +2837,7 @@
         <v>1202</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2875,7 +2856,7 @@
         <v>1203</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2894,7 +2875,7 @@
         <v>1204</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2913,7 +2894,7 @@
         <v>1205</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2932,7 +2913,7 @@
         <v>1206</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2951,7 +2932,7 @@
         <v>1207</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>521</v>
+        <v>504</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2970,7 +2951,7 @@
         <v>1208</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2989,7 +2970,7 @@
         <v>1209</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>508</v>
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,7 +2989,7 @@
         <v>1300</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>535</v>
+        <v>518</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3027,7 +3008,7 @@
         <v>1301</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3027,7 @@
         <v>1302</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3065,7 +3046,7 @@
         <v>1400</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>536</v>
+        <v>519</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3084,7 +3065,7 @@
         <v>1401</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>525</v>
+        <v>508</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3103,7 +3084,7 @@
         <v>1402</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3122,7 +3103,7 @@
         <v>1403</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>527</v>
+        <v>510</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3141,7 +3122,7 @@
         <v>1500</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>537</v>
+        <v>520</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3160,7 +3141,7 @@
         <v>1501</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3179,7 +3160,7 @@
         <v>1502</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3198,7 +3179,7 @@
         <v>1503</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3217,7 +3198,7 @@
         <v>1504</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3236,7 +3217,7 @@
         <v>1505</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3255,7 +3236,7 @@
         <v>1600</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3274,7 +3255,7 @@
         <v>1601</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -3293,7 +3274,7 @@
         <v>1602</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -3312,7 +3293,7 @@
         <v>1800</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>539</v>
+        <v>522</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -3331,7 +3312,7 @@
         <v>1801</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>543</v>
+        <v>526</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3350,7 +3331,7 @@
         <v>1802</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>544</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -3374,42 +3355,42 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3422,8 +3403,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,7 +3441,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>165</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3471,7 +3452,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>166</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3482,7 +3463,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>167</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3493,7 +3474,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>168</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3504,7 +3485,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>169</v>
+        <v>549</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3515,7 +3496,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>451</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3526,7 +3507,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3537,7 +3518,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3548,7 +3529,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3559,7 +3540,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3570,7 +3551,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3581,7 +3562,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3592,7 +3573,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3603,7 +3584,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3614,7 +3595,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3625,7 +3606,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3636,7 +3617,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3647,7 +3628,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>446</v>
+        <v>545</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3658,7 +3639,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3669,7 +3650,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>454</v>
+        <v>544</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3680,7 +3661,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3691,7 +3672,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3702,7 +3683,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3713,7 +3694,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3724,7 +3705,7 @@
         <v>162</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3735,7 +3716,7 @@
         <v>162</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3746,7 +3727,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3757,7 +3738,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>458</v>
+        <v>441</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3768,7 +3749,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3779,7 +3760,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3790,7 +3771,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3801,7 +3782,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3812,7 +3793,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3823,7 +3804,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3834,7 +3815,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3845,7 +3826,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3856,7 +3837,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3867,7 +3848,7 @@
         <v>162</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3878,7 +3859,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3889,7 +3870,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3900,7 +3881,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -3911,7 +3892,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3922,7 +3903,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3933,7 +3914,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3944,7 +3925,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3955,7 +3936,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3966,7 +3947,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3977,7 +3958,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3988,7 +3969,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3999,7 +3980,7 @@
         <v>162</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4010,7 +3991,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4021,7 +4002,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -4032,7 +4013,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -4043,7 +4024,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4054,7 +4035,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -4065,7 +4046,7 @@
         <v>162</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -4076,7 +4057,7 @@
         <v>162</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -4087,7 +4068,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -4098,7 +4079,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -4109,7 +4090,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -4120,7 +4101,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4131,7 +4112,7 @@
         <v>162</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4142,7 +4123,7 @@
         <v>162</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -4153,7 +4134,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -4164,7 +4145,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4175,7 +4156,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4186,7 +4167,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -4197,7 +4178,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4208,7 +4189,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -4219,7 +4200,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -4230,7 +4211,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -4241,7 +4222,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4252,7 +4233,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -4263,7 +4244,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -4274,7 +4255,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -4285,7 +4266,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -4296,7 +4277,7 @@
         <v>162</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -4307,7 +4288,7 @@
         <v>162</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -4318,7 +4299,7 @@
         <v>162</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -4329,7 +4310,7 @@
         <v>162</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -4340,7 +4321,7 @@
         <v>162</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -4351,7 +4332,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -4362,7 +4343,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -4373,7 +4354,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -4384,7 +4365,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -4395,7 +4376,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -4406,7 +4387,7 @@
         <v>162</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -4417,7 +4398,7 @@
         <v>162</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -4428,7 +4409,7 @@
         <v>162</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -4439,7 +4420,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>560</v>
+        <v>542</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -4450,7 +4431,7 @@
         <v>162</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -4461,7 +4442,7 @@
         <v>162</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -4472,7 +4453,7 @@
         <v>162</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -4483,7 +4464,7 @@
         <v>162</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -4494,7 +4475,7 @@
         <v>162</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -4505,7 +4486,7 @@
         <v>162</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -4516,7 +4497,7 @@
         <v>162</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -4527,7 +4508,7 @@
         <v>162</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -4538,7 +4519,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -4549,7 +4530,7 @@
         <v>162</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -4560,7 +4541,7 @@
         <v>162</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -4571,7 +4552,7 @@
         <v>162</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -4582,7 +4563,7 @@
         <v>162</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -4593,7 +4574,7 @@
         <v>162</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -4604,7 +4585,7 @@
         <v>162</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -4615,7 +4596,7 @@
         <v>162</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4626,7 +4607,7 @@
         <v>162</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4637,7 +4618,7 @@
         <v>162</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -4648,7 +4629,7 @@
         <v>162</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -4659,7 +4640,7 @@
         <v>162</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -4670,7 +4651,7 @@
         <v>162</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -4681,7 +4662,7 @@
         <v>162</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -4692,7 +4673,7 @@
         <v>162</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -4703,7 +4684,7 @@
         <v>162</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -4714,7 +4695,7 @@
         <v>162</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -4725,7 +4706,7 @@
         <v>162</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -4736,7 +4717,7 @@
         <v>162</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -4747,7 +4728,7 @@
         <v>162</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -4758,7 +4739,7 @@
         <v>162</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -4769,7 +4750,7 @@
         <v>162</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -4780,7 +4761,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>547</v>
+        <v>530</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4791,7 +4772,7 @@
         <v>162</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>546</v>
+        <v>529</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4802,7 +4783,7 @@
         <v>162</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -4813,7 +4794,7 @@
         <v>162</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -4824,7 +4805,7 @@
         <v>162</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -4835,7 +4816,7 @@
         <v>162</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -4846,7 +4827,7 @@
         <v>162</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -4857,7 +4838,7 @@
         <v>162</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -4868,7 +4849,7 @@
         <v>162</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4879,7 +4860,7 @@
         <v>162</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -4890,7 +4871,7 @@
         <v>162</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -4901,7 +4882,7 @@
         <v>162</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -4912,7 +4893,7 @@
         <v>162</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -4923,7 +4904,7 @@
         <v>162</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -4934,7 +4915,7 @@
         <v>162</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -4945,7 +4926,7 @@
         <v>162</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -4956,7 +4937,7 @@
         <v>162</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -4967,7 +4948,7 @@
         <v>162</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -4978,7 +4959,7 @@
         <v>162</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4989,7 +4970,7 @@
         <v>162</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -5000,7 +4981,7 @@
         <v>162</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -5011,7 +4992,7 @@
         <v>162</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -5022,7 +5003,7 @@
         <v>162</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -5033,7 +5014,7 @@
         <v>162</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -5044,7 +5025,7 @@
         <v>162</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -5055,7 +5036,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -5066,7 +5047,7 @@
         <v>162</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -5077,7 +5058,7 @@
         <v>162</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -5088,7 +5069,7 @@
         <v>162</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -5099,7 +5080,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>503</v>
+        <v>486</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -5110,7 +5091,7 @@
         <v>162</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -5121,7 +5102,7 @@
         <v>162</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -5132,7 +5113,7 @@
         <v>162</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -5143,7 +5124,7 @@
         <v>162</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -5154,7 +5135,7 @@
         <v>162</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -5165,7 +5146,7 @@
         <v>162</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -5176,7 +5157,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>556</v>
+        <v>539</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -5187,7 +5168,7 @@
         <v>162</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -5198,7 +5179,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -5209,7 +5190,7 @@
         <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -5220,7 +5201,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -5231,194 +5212,194 @@
         <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
-        <v>548</v>
+        <v>531</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
-        <v>550</v>
+        <v>533</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -5433,8 +5414,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5446,7 +5427,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5471,7 +5452,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5482,7 +5463,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5493,7 +5474,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>220</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5504,7 +5485,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5515,7 +5496,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5526,7 +5507,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>220</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5537,7 +5518,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5548,7 +5529,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5559,7 +5540,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5570,7 +5551,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5581,7 +5562,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5592,7 +5573,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5603,7 +5584,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5614,7 +5595,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5625,7 +5606,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5636,7 +5617,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5647,7 +5628,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5658,7 +5639,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5669,7 +5650,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5680,7 +5661,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5691,7 +5672,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5702,7 +5683,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5713,7 +5694,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5724,7 +5705,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5735,7 +5716,7 @@
         <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5746,7 +5727,7 @@
         <v>162</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5757,7 +5738,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5768,7 +5749,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5779,7 +5760,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5790,7 +5771,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5801,7 +5782,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5812,7 +5793,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5823,7 +5804,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5834,7 +5815,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5845,7 +5826,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5856,7 +5837,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5867,7 +5848,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5878,7 +5859,7 @@
         <v>162</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5889,7 +5870,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5900,7 +5881,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5911,7 +5892,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5922,7 +5903,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5933,7 +5914,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5944,7 +5925,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5955,7 +5936,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5966,7 +5947,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5977,7 +5958,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5988,7 +5969,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5999,7 +5980,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6010,7 +5991,7 @@
         <v>162</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6021,7 +6002,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6032,7 +6013,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6043,7 +6024,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6054,7 +6035,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6065,7 +6046,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6172,7 +6153,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6183,7 +6164,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6194,7 +6175,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6205,7 +6186,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6216,7 +6197,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6227,7 +6208,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6238,7 +6219,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6249,7 +6230,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6260,7 +6241,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6271,7 +6252,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6282,7 +6263,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6293,7 +6274,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6304,7 +6285,7 @@
         <v>162</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6315,7 +6296,7 @@
         <v>162</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -6326,7 +6307,7 @@
         <v>162</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6337,7 +6318,7 @@
         <v>162</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6348,7 +6329,7 @@
         <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -6359,7 +6340,7 @@
         <v>162</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6370,7 +6351,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -6381,7 +6362,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6392,7 +6373,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6403,7 +6384,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6414,7 +6395,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -6425,7 +6406,7 @@
         <v>162</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6436,7 +6417,7 @@
         <v>162</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6447,7 +6428,7 @@
         <v>162</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -6458,7 +6439,7 @@
         <v>162</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>501</v>
+        <v>484</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6469,7 +6450,7 @@
         <v>162</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6480,7 +6461,7 @@
         <v>162</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6491,7 +6472,7 @@
         <v>162</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6502,7 +6483,7 @@
         <v>162</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6609,7 +6590,7 @@
         <v>162</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -6620,7 +6601,7 @@
         <v>162</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -6631,7 +6612,7 @@
         <v>162</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -6642,7 +6623,7 @@
         <v>162</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -6653,7 +6634,7 @@
         <v>162</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -6664,7 +6645,7 @@
         <v>162</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -6675,7 +6656,7 @@
         <v>162</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -6686,7 +6667,7 @@
         <v>162</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -6701,8 +6682,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6714,7 +6695,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6739,7 +6720,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6750,7 +6731,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6761,7 +6742,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6772,7 +6753,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>298</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6783,7 +6764,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>297</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6794,7 +6775,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6805,7 +6786,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6816,7 +6797,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6827,7 +6808,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6838,7 +6819,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6849,7 +6830,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6860,7 +6841,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6871,7 +6852,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6882,7 +6863,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6893,7 +6874,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6904,7 +6885,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6915,7 +6896,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6926,7 +6907,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6937,7 +6918,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6948,7 +6929,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6959,7 +6940,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6970,7 +6951,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6981,7 +6962,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6992,7 +6973,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -7003,7 +6984,7 @@
         <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -7014,7 +6995,7 @@
         <v>162</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -7025,7 +7006,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -7036,7 +7017,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -7047,7 +7028,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -7058,7 +7039,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -7069,7 +7050,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -7080,7 +7061,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -7091,7 +7072,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -7102,7 +7083,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -7113,7 +7094,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -7124,7 +7105,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>286</v>
+        <v>543</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -7135,7 +7116,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -7146,7 +7127,7 @@
         <v>162</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -7157,7 +7138,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -7168,7 +7149,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -7179,7 +7160,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -7190,7 +7171,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -7201,7 +7182,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -7212,7 +7193,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -7223,7 +7204,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -7234,7 +7215,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -7245,7 +7226,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -7256,7 +7237,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -7267,7 +7248,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -7278,7 +7259,7 @@
         <v>162</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -7289,7 +7270,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -7300,7 +7281,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -7311,7 +7292,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -7322,7 +7303,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -7333,7 +7314,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -7344,7 +7325,7 @@
         <v>162</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -7355,10 +7336,10 @@
         <v>162</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="D59" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -7369,7 +7350,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -7380,7 +7361,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -7391,7 +7372,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -7402,7 +7383,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -7413,10 +7394,10 @@
         <v>162</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="D64" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -7427,7 +7408,7 @@
         <v>162</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -7438,7 +7419,7 @@
         <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -7449,7 +7430,7 @@
         <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -7460,7 +7441,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -7471,7 +7452,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -7482,7 +7463,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -7493,7 +7474,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -7504,7 +7485,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -7515,7 +7496,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -7622,7 +7603,7 @@
         <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -7633,7 +7614,7 @@
         <v>162</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -7644,7 +7625,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -7655,7 +7636,7 @@
         <v>162</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -7666,7 +7647,7 @@
         <v>162</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -7677,7 +7658,7 @@
         <v>162</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -7688,7 +7669,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -7713,7 +7694,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7732,13 +7713,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -7751,7 +7732,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
@@ -7764,7 +7745,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7789,7 +7770,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -7800,7 +7781,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -7811,7 +7792,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -7822,7 +7803,7 @@
         <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -7833,7 +7814,7 @@
         <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7844,7 +7825,7 @@
         <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -7855,7 +7836,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7866,7 +7847,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -7877,7 +7858,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -7888,7 +7869,7 @@
         <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -7899,7 +7880,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -7910,7 +7891,7 @@
         <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -7921,7 +7902,7 @@
         <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -7932,7 +7913,7 @@
         <v>162</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7943,7 +7924,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -7954,7 +7935,7 @@
         <v>162</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -7965,7 +7946,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -7976,7 +7957,7 @@
         <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -7987,7 +7968,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -7998,7 +7979,7 @@
         <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -8009,7 +7990,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -8020,7 +8001,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -8031,7 +8012,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -8042,7 +8023,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -8053,7 +8034,7 @@
         <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -8064,7 +8045,7 @@
         <v>162</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -8075,7 +8056,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -8086,7 +8067,7 @@
         <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -8097,7 +8078,7 @@
         <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -8108,7 +8089,7 @@
         <v>162</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -8119,7 +8100,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -8130,7 +8111,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -8141,7 +8122,7 @@
         <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -8152,7 +8133,7 @@
         <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -8163,7 +8144,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -8174,7 +8155,7 @@
         <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -8185,7 +8166,7 @@
         <v>162</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -8196,7 +8177,7 @@
         <v>162</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -8207,7 +8188,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -8218,7 +8199,7 @@
         <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -8229,7 +8210,7 @@
         <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -8240,7 +8221,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -8251,7 +8232,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -8262,7 +8243,7 @@
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -8273,7 +8254,7 @@
         <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -8284,7 +8265,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -8295,7 +8276,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -8306,7 +8287,7 @@
         <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -8317,7 +8298,7 @@
         <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -8328,7 +8309,7 @@
         <v>162</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -8339,7 +8320,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -8350,7 +8331,7 @@
         <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -8361,7 +8342,7 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -8372,7 +8353,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -8383,7 +8364,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -8394,7 +8375,7 @@
         <v>162</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -8405,7 +8386,7 @@
         <v>162</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -8416,7 +8397,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -8523,7 +8504,7 @@
         <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -8534,7 +8515,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -8545,7 +8526,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -8556,7 +8537,7 @@
         <v>162</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -8567,7 +8548,7 @@
         <v>162</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -8578,7 +8559,7 @@
         <v>162</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -8589,7 +8570,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -8600,7 +8581,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -8611,7 +8592,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>